<commit_message>
update instruction job/split sur OT
</commit_message>
<xml_diff>
--- a/lib/PHPExcel/templates/OT_LoS.xlsx
+++ b/lib/PHPExcel/templates/OT_LoS.xlsx
@@ -683,22 +683,26 @@
     <xf numFmtId="167" fontId="10" fillId="4" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="40" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -712,30 +716,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="40" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="40" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="40" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Milliers 2" xfId="1"/>
@@ -1525,10 +1525,10 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="64" t="s">
+      <c r="J2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="65"/>
+      <c r="K2" s="81"/>
       <c r="L2" s="71"/>
       <c r="M2" s="72"/>
       <c r="N2" s="1"/>
@@ -1537,10 +1537,10 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
-      <c r="T2" s="64" t="s">
+      <c r="T2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="80"/>
+      <c r="U2" s="68"/>
       <c r="V2" s="71" t="str">
         <f t="shared" ref="V2:V3" si="0">IF(ISBLANK(L2),"",L2)</f>
         <v/>
@@ -1552,10 +1552,10 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
       <c r="AC2" s="1"/>
-      <c r="AD2" s="64" t="s">
+      <c r="AD2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="80"/>
+      <c r="AE2" s="68"/>
       <c r="AF2" s="71" t="str">
         <f t="shared" ref="AF2:AF3" si="1">IF(ISBLANK(V2),"",V2)</f>
         <v/>
@@ -1567,10 +1567,10 @@
       <c r="AK2" s="1"/>
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
-      <c r="AN2" s="64" t="s">
+      <c r="AN2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AO2" s="80"/>
+      <c r="AO2" s="68"/>
       <c r="AP2" s="71" t="str">
         <f t="shared" ref="AP2:AP3" si="2">IF(ISBLANK(AF2),"",AF2)</f>
         <v/>
@@ -1582,10 +1582,10 @@
       <c r="AU2" s="1"/>
       <c r="AV2" s="1"/>
       <c r="AW2" s="1"/>
-      <c r="AX2" s="64" t="s">
+      <c r="AX2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="AY2" s="80"/>
+      <c r="AY2" s="68"/>
       <c r="AZ2" s="71" t="str">
         <f t="shared" ref="AZ2:AZ3" si="3">IF(ISBLANK(AP2),"",AP2)</f>
         <v/>
@@ -1597,10 +1597,10 @@
       <c r="BE2" s="1"/>
       <c r="BF2" s="1"/>
       <c r="BG2" s="1"/>
-      <c r="BH2" s="64" t="s">
+      <c r="BH2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="BI2" s="80"/>
+      <c r="BI2" s="68"/>
       <c r="BJ2" s="71" t="str">
         <f t="shared" ref="BJ2:BJ3" si="4">IF(ISBLANK(AZ2),"",AZ2)</f>
         <v/>
@@ -1612,10 +1612,10 @@
       <c r="BO2" s="1"/>
       <c r="BP2" s="1"/>
       <c r="BQ2" s="1"/>
-      <c r="BR2" s="64" t="s">
+      <c r="BR2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="BS2" s="80"/>
+      <c r="BS2" s="68"/>
       <c r="BT2" s="71" t="str">
         <f t="shared" ref="BT2:BT3" si="5">IF(ISBLANK(BJ2),"",BJ2)</f>
         <v/>
@@ -1627,10 +1627,10 @@
       <c r="BY2" s="1"/>
       <c r="BZ2" s="1"/>
       <c r="CA2" s="1"/>
-      <c r="CB2" s="64" t="s">
+      <c r="CB2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="CC2" s="80"/>
+      <c r="CC2" s="68"/>
       <c r="CD2" s="71" t="str">
         <f t="shared" ref="CD2:CD3" si="6">IF(ISBLANK(BT2),"",BT2)</f>
         <v/>
@@ -1642,10 +1642,10 @@
       <c r="CI2" s="1"/>
       <c r="CJ2" s="1"/>
       <c r="CK2" s="1"/>
-      <c r="CL2" s="64" t="s">
+      <c r="CL2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="CM2" s="80"/>
+      <c r="CM2" s="68"/>
       <c r="CN2" s="71" t="str">
         <f t="shared" ref="CN2:CN3" si="7">IF(ISBLANK(CD2),"",CD2)</f>
         <v/>
@@ -1657,10 +1657,10 @@
       <c r="CS2" s="1"/>
       <c r="CT2" s="1"/>
       <c r="CU2" s="1"/>
-      <c r="CV2" s="64" t="s">
+      <c r="CV2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="CW2" s="80"/>
+      <c r="CW2" s="68"/>
       <c r="CX2" s="71" t="str">
         <f t="shared" ref="CX2:CX3" si="8">IF(ISBLANK(CN2),"",CN2)</f>
         <v/>
@@ -1672,10 +1672,10 @@
       <c r="DC2" s="1"/>
       <c r="DD2" s="1"/>
       <c r="DE2" s="1"/>
-      <c r="DF2" s="64" t="s">
+      <c r="DF2" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="DG2" s="80"/>
+      <c r="DG2" s="68"/>
       <c r="DH2" s="71" t="str">
         <f t="shared" ref="DH2:DH3" si="9">IF(ISBLANK(CX2),"",CX2)</f>
         <v/>
@@ -1692,8 +1692,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="67"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="82"/>
       <c r="L3" s="73"/>
       <c r="M3" s="74"/>
       <c r="N3" s="1"/>
@@ -1702,8 +1702,8 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
-      <c r="T3" s="66"/>
-      <c r="U3" s="81"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="70"/>
       <c r="V3" s="73" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1715,8 +1715,8 @@
       <c r="AA3" s="1"/>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1"/>
-      <c r="AD3" s="66"/>
-      <c r="AE3" s="81"/>
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="70"/>
       <c r="AF3" s="73" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -1728,8 +1728,8 @@
       <c r="AK3" s="1"/>
       <c r="AL3" s="1"/>
       <c r="AM3" s="1"/>
-      <c r="AN3" s="66"/>
-      <c r="AO3" s="81"/>
+      <c r="AN3" s="69"/>
+      <c r="AO3" s="70"/>
       <c r="AP3" s="73" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1741,8 +1741,8 @@
       <c r="AU3" s="1"/>
       <c r="AV3" s="1"/>
       <c r="AW3" s="1"/>
-      <c r="AX3" s="66"/>
-      <c r="AY3" s="81"/>
+      <c r="AX3" s="69"/>
+      <c r="AY3" s="70"/>
       <c r="AZ3" s="73" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -1754,8 +1754,8 @@
       <c r="BE3" s="1"/>
       <c r="BF3" s="1"/>
       <c r="BG3" s="1"/>
-      <c r="BH3" s="66"/>
-      <c r="BI3" s="81"/>
+      <c r="BH3" s="69"/>
+      <c r="BI3" s="70"/>
       <c r="BJ3" s="73" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -1767,8 +1767,8 @@
       <c r="BO3" s="1"/>
       <c r="BP3" s="1"/>
       <c r="BQ3" s="1"/>
-      <c r="BR3" s="66"/>
-      <c r="BS3" s="81"/>
+      <c r="BR3" s="69"/>
+      <c r="BS3" s="70"/>
       <c r="BT3" s="73" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -1780,8 +1780,8 @@
       <c r="BY3" s="1"/>
       <c r="BZ3" s="1"/>
       <c r="CA3" s="1"/>
-      <c r="CB3" s="66"/>
-      <c r="CC3" s="81"/>
+      <c r="CB3" s="69"/>
+      <c r="CC3" s="70"/>
       <c r="CD3" s="73" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -1793,8 +1793,8 @@
       <c r="CI3" s="1"/>
       <c r="CJ3" s="1"/>
       <c r="CK3" s="1"/>
-      <c r="CL3" s="66"/>
-      <c r="CM3" s="81"/>
+      <c r="CL3" s="69"/>
+      <c r="CM3" s="70"/>
       <c r="CN3" s="73" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -1806,8 +1806,8 @@
       <c r="CS3" s="1"/>
       <c r="CT3" s="1"/>
       <c r="CU3" s="1"/>
-      <c r="CV3" s="66"/>
-      <c r="CW3" s="81"/>
+      <c r="CV3" s="69"/>
+      <c r="CW3" s="70"/>
       <c r="CX3" s="73" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -1819,8 +1819,8 @@
       <c r="DC3" s="1"/>
       <c r="DD3" s="1"/>
       <c r="DE3" s="1"/>
-      <c r="DF3" s="66"/>
-      <c r="DG3" s="81"/>
+      <c r="DF3" s="69"/>
+      <c r="DG3" s="70"/>
       <c r="DH3" s="73" t="str">
         <f t="shared" si="9"/>
         <v/>
@@ -1838,214 +1838,214 @@
         <v>0</v>
       </c>
       <c r="F4" s="1"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="69"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="80"/>
       <c r="I4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="J4" s="1"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
+      <c r="K4" s="76"/>
+      <c r="L4" s="76"/>
       <c r="M4" s="6"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P4" s="1"/>
-      <c r="Q4" s="68" t="str">
+      <c r="Q4" s="75" t="str">
         <f>IF(ISBLANK(G4),"",G4)</f>
         <v/>
       </c>
-      <c r="R4" s="68"/>
+      <c r="R4" s="75"/>
       <c r="S4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="T4" s="1"/>
-      <c r="U4" s="70" t="str">
+      <c r="U4" s="76" t="str">
         <f t="shared" ref="U4:U6" si="10">IF(ISBLANK(K4),"",K4)</f>
         <v/>
       </c>
-      <c r="V4" s="70"/>
+      <c r="V4" s="76"/>
       <c r="W4" s="6"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z4" s="1"/>
-      <c r="AA4" s="68" t="str">
+      <c r="AA4" s="75" t="str">
         <f>IF(ISBLANK(Q4),"",Q4)</f>
         <v/>
       </c>
-      <c r="AB4" s="68"/>
+      <c r="AB4" s="75"/>
       <c r="AC4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AD4" s="1"/>
-      <c r="AE4" s="70" t="str">
+      <c r="AE4" s="76" t="str">
         <f t="shared" ref="AE4:AE6" si="11">IF(ISBLANK(U4),"",U4)</f>
         <v/>
       </c>
-      <c r="AF4" s="70"/>
+      <c r="AF4" s="76"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AJ4" s="1"/>
-      <c r="AK4" s="68" t="str">
+      <c r="AK4" s="75" t="str">
         <f>IF(ISBLANK(AA4),"",AA4)</f>
         <v/>
       </c>
-      <c r="AL4" s="68"/>
+      <c r="AL4" s="75"/>
       <c r="AM4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AN4" s="1"/>
-      <c r="AO4" s="70" t="str">
+      <c r="AO4" s="76" t="str">
         <f t="shared" ref="AO4:AO6" si="12">IF(ISBLANK(AE4),"",AE4)</f>
         <v/>
       </c>
-      <c r="AP4" s="70"/>
+      <c r="AP4" s="76"/>
       <c r="AQ4" s="6"/>
       <c r="AR4" s="1"/>
       <c r="AS4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AT4" s="1"/>
-      <c r="AU4" s="68" t="str">
+      <c r="AU4" s="75" t="str">
         <f>IF(ISBLANK(AK4),"",AK4)</f>
         <v/>
       </c>
-      <c r="AV4" s="68"/>
+      <c r="AV4" s="75"/>
       <c r="AW4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="AX4" s="1"/>
-      <c r="AY4" s="70" t="str">
+      <c r="AY4" s="76" t="str">
         <f t="shared" ref="AY4:AY6" si="13">IF(ISBLANK(AO4),"",AO4)</f>
         <v/>
       </c>
-      <c r="AZ4" s="70"/>
+      <c r="AZ4" s="76"/>
       <c r="BA4" s="6"/>
       <c r="BB4" s="1"/>
       <c r="BC4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="BD4" s="1"/>
-      <c r="BE4" s="68" t="str">
+      <c r="BE4" s="75" t="str">
         <f>IF(ISBLANK(AU4),"",AU4)</f>
         <v/>
       </c>
-      <c r="BF4" s="68"/>
+      <c r="BF4" s="75"/>
       <c r="BG4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="BH4" s="1"/>
-      <c r="BI4" s="70" t="str">
+      <c r="BI4" s="76" t="str">
         <f t="shared" ref="BI4:BI6" si="14">IF(ISBLANK(AY4),"",AY4)</f>
         <v/>
       </c>
-      <c r="BJ4" s="70"/>
+      <c r="BJ4" s="76"/>
       <c r="BK4" s="6"/>
       <c r="BL4" s="1"/>
       <c r="BM4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="BN4" s="1"/>
-      <c r="BO4" s="68" t="str">
+      <c r="BO4" s="75" t="str">
         <f>IF(ISBLANK(BE4),"",BE4)</f>
         <v/>
       </c>
-      <c r="BP4" s="68"/>
+      <c r="BP4" s="75"/>
       <c r="BQ4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="BR4" s="1"/>
-      <c r="BS4" s="70" t="str">
+      <c r="BS4" s="76" t="str">
         <f t="shared" ref="BS4:BS6" si="15">IF(ISBLANK(BI4),"",BI4)</f>
         <v/>
       </c>
-      <c r="BT4" s="70"/>
+      <c r="BT4" s="76"/>
       <c r="BU4" s="6"/>
       <c r="BV4" s="1"/>
       <c r="BW4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="BX4" s="1"/>
-      <c r="BY4" s="68" t="str">
+      <c r="BY4" s="75" t="str">
         <f>IF(ISBLANK(BO4),"",BO4)</f>
         <v/>
       </c>
-      <c r="BZ4" s="68"/>
+      <c r="BZ4" s="75"/>
       <c r="CA4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="CB4" s="1"/>
-      <c r="CC4" s="70" t="str">
+      <c r="CC4" s="76" t="str">
         <f t="shared" ref="CC4:CC6" si="16">IF(ISBLANK(BS4),"",BS4)</f>
         <v/>
       </c>
-      <c r="CD4" s="70"/>
+      <c r="CD4" s="76"/>
       <c r="CE4" s="6"/>
       <c r="CF4" s="1"/>
       <c r="CG4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="CH4" s="1"/>
-      <c r="CI4" s="68" t="str">
+      <c r="CI4" s="75" t="str">
         <f>IF(ISBLANK(BY4),"",BY4)</f>
         <v/>
       </c>
-      <c r="CJ4" s="68"/>
+      <c r="CJ4" s="75"/>
       <c r="CK4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="CL4" s="1"/>
-      <c r="CM4" s="70" t="str">
+      <c r="CM4" s="76" t="str">
         <f t="shared" ref="CM4:CM6" si="17">IF(ISBLANK(CC4),"",CC4)</f>
         <v/>
       </c>
-      <c r="CN4" s="70"/>
+      <c r="CN4" s="76"/>
       <c r="CO4" s="6"/>
       <c r="CP4" s="1"/>
       <c r="CQ4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="CR4" s="1"/>
-      <c r="CS4" s="68" t="str">
+      <c r="CS4" s="75" t="str">
         <f>IF(ISBLANK(CI4),"",CI4)</f>
         <v/>
       </c>
-      <c r="CT4" s="68"/>
+      <c r="CT4" s="75"/>
       <c r="CU4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="CV4" s="1"/>
-      <c r="CW4" s="70" t="str">
+      <c r="CW4" s="76" t="str">
         <f t="shared" ref="CW4:CW6" si="18">IF(ISBLANK(CM4),"",CM4)</f>
         <v/>
       </c>
-      <c r="CX4" s="70"/>
+      <c r="CX4" s="76"/>
       <c r="CY4" s="6"/>
       <c r="CZ4" s="1"/>
       <c r="DA4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="DB4" s="1"/>
-      <c r="DC4" s="68" t="str">
+      <c r="DC4" s="75" t="str">
         <f>IF(ISBLANK(CS4),"",CS4)</f>
         <v/>
       </c>
-      <c r="DD4" s="68"/>
+      <c r="DD4" s="75"/>
       <c r="DE4" s="1" t="s">
         <v>26</v>
       </c>
       <c r="DF4" s="1"/>
-      <c r="DG4" s="70" t="str">
+      <c r="DG4" s="76" t="str">
         <f t="shared" ref="DG4:DG6" si="19">IF(ISBLANK(CW4),"",CW4)</f>
         <v/>
       </c>
-      <c r="DH4" s="70"/>
+      <c r="DH4" s="76"/>
       <c r="DI4" s="6"/>
     </row>
     <row r="5" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2057,14 +2057,14 @@
         <v>1</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="69"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="80"/>
       <c r="I5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
+      <c r="K5" s="80"/>
+      <c r="L5" s="80"/>
       <c r="M5" s="6"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1" t="s">
@@ -2080,11 +2080,11 @@
         <v>19</v>
       </c>
       <c r="T5" s="1"/>
-      <c r="U5" s="78" t="str">
+      <c r="U5" s="66" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="V5" s="78"/>
+      <c r="V5" s="66"/>
       <c r="W5" s="6"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1" t="s">
@@ -2100,11 +2100,11 @@
         <v>19</v>
       </c>
       <c r="AD5" s="1"/>
-      <c r="AE5" s="78" t="str">
+      <c r="AE5" s="66" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AF5" s="78"/>
+      <c r="AF5" s="66"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1" t="s">
@@ -2120,11 +2120,11 @@
         <v>19</v>
       </c>
       <c r="AN5" s="1"/>
-      <c r="AO5" s="78" t="str">
+      <c r="AO5" s="66" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AP5" s="78"/>
+      <c r="AP5" s="66"/>
       <c r="AQ5" s="6"/>
       <c r="AR5" s="1"/>
       <c r="AS5" s="1" t="s">
@@ -2140,11 +2140,11 @@
         <v>19</v>
       </c>
       <c r="AX5" s="1"/>
-      <c r="AY5" s="78" t="str">
+      <c r="AY5" s="66" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AZ5" s="78"/>
+      <c r="AZ5" s="66"/>
       <c r="BA5" s="6"/>
       <c r="BB5" s="1"/>
       <c r="BC5" s="1" t="s">
@@ -2160,11 +2160,11 @@
         <v>19</v>
       </c>
       <c r="BH5" s="1"/>
-      <c r="BI5" s="78" t="str">
+      <c r="BI5" s="66" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="BJ5" s="78"/>
+      <c r="BJ5" s="66"/>
       <c r="BK5" s="6"/>
       <c r="BL5" s="1"/>
       <c r="BM5" s="1" t="s">
@@ -2180,11 +2180,11 @@
         <v>19</v>
       </c>
       <c r="BR5" s="1"/>
-      <c r="BS5" s="78" t="str">
+      <c r="BS5" s="66" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="BT5" s="78"/>
+      <c r="BT5" s="66"/>
       <c r="BU5" s="6"/>
       <c r="BV5" s="1"/>
       <c r="BW5" s="1" t="s">
@@ -2200,11 +2200,11 @@
         <v>19</v>
       </c>
       <c r="CB5" s="1"/>
-      <c r="CC5" s="78" t="str">
+      <c r="CC5" s="66" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="CD5" s="78"/>
+      <c r="CD5" s="66"/>
       <c r="CE5" s="6"/>
       <c r="CF5" s="1"/>
       <c r="CG5" s="1" t="s">
@@ -2220,11 +2220,11 @@
         <v>19</v>
       </c>
       <c r="CL5" s="1"/>
-      <c r="CM5" s="78" t="str">
+      <c r="CM5" s="66" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="CN5" s="78"/>
+      <c r="CN5" s="66"/>
       <c r="CO5" s="6"/>
       <c r="CP5" s="1"/>
       <c r="CQ5" s="1" t="s">
@@ -2240,11 +2240,11 @@
         <v>19</v>
       </c>
       <c r="CV5" s="1"/>
-      <c r="CW5" s="78" t="str">
+      <c r="CW5" s="66" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="CX5" s="78"/>
+      <c r="CX5" s="66"/>
       <c r="CY5" s="6"/>
       <c r="CZ5" s="1"/>
       <c r="DA5" s="1" t="s">
@@ -2260,11 +2260,11 @@
         <v>19</v>
       </c>
       <c r="DF5" s="1"/>
-      <c r="DG5" s="78" t="str">
+      <c r="DG5" s="66" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
-      <c r="DH5" s="78"/>
+      <c r="DH5" s="66"/>
       <c r="DI5" s="6"/>
     </row>
     <row r="6" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2278,214 +2278,214 @@
         <v>2</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="78"/>
       <c r="I6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="1"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
       <c r="M6" s="6"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="P6" s="1"/>
-      <c r="Q6" s="79" t="str">
+      <c r="Q6" s="65" t="str">
         <f t="shared" si="20"/>
         <v/>
       </c>
-      <c r="R6" s="79"/>
+      <c r="R6" s="65"/>
       <c r="S6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T6" s="1"/>
-      <c r="U6" s="78" t="str">
+      <c r="U6" s="66" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="V6" s="78"/>
+      <c r="V6" s="66"/>
       <c r="W6" s="6"/>
       <c r="X6" s="1"/>
       <c r="Y6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="Z6" s="1"/>
-      <c r="AA6" s="79" t="str">
+      <c r="AA6" s="65" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="AB6" s="79"/>
+      <c r="AB6" s="65"/>
       <c r="AC6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AD6" s="1"/>
-      <c r="AE6" s="78" t="str">
+      <c r="AE6" s="66" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
-      <c r="AF6" s="78"/>
+      <c r="AF6" s="66"/>
       <c r="AG6" s="6"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AJ6" s="1"/>
-      <c r="AK6" s="79" t="str">
+      <c r="AK6" s="65" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="AL6" s="79"/>
+      <c r="AL6" s="65"/>
       <c r="AM6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AN6" s="1"/>
-      <c r="AO6" s="78" t="str">
+      <c r="AO6" s="66" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="AP6" s="78"/>
+      <c r="AP6" s="66"/>
       <c r="AQ6" s="6"/>
       <c r="AR6" s="1"/>
       <c r="AS6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AT6" s="1"/>
-      <c r="AU6" s="79" t="str">
+      <c r="AU6" s="65" t="str">
         <f t="shared" si="23"/>
         <v/>
       </c>
-      <c r="AV6" s="79"/>
+      <c r="AV6" s="65"/>
       <c r="AW6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AX6" s="1"/>
-      <c r="AY6" s="78" t="str">
+      <c r="AY6" s="66" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
-      <c r="AZ6" s="78"/>
+      <c r="AZ6" s="66"/>
       <c r="BA6" s="6"/>
       <c r="BB6" s="1"/>
       <c r="BC6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="BD6" s="1"/>
-      <c r="BE6" s="79" t="str">
+      <c r="BE6" s="65" t="str">
         <f t="shared" si="24"/>
         <v/>
       </c>
-      <c r="BF6" s="79"/>
+      <c r="BF6" s="65"/>
       <c r="BG6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="BH6" s="1"/>
-      <c r="BI6" s="78" t="str">
+      <c r="BI6" s="66" t="str">
         <f t="shared" si="14"/>
         <v/>
       </c>
-      <c r="BJ6" s="78"/>
+      <c r="BJ6" s="66"/>
       <c r="BK6" s="6"/>
       <c r="BL6" s="1"/>
       <c r="BM6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="BN6" s="1"/>
-      <c r="BO6" s="79" t="str">
+      <c r="BO6" s="65" t="str">
         <f t="shared" si="25"/>
         <v/>
       </c>
-      <c r="BP6" s="79"/>
+      <c r="BP6" s="65"/>
       <c r="BQ6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="BR6" s="1"/>
-      <c r="BS6" s="78" t="str">
+      <c r="BS6" s="66" t="str">
         <f t="shared" si="15"/>
         <v/>
       </c>
-      <c r="BT6" s="78"/>
+      <c r="BT6" s="66"/>
       <c r="BU6" s="6"/>
       <c r="BV6" s="1"/>
       <c r="BW6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="BX6" s="1"/>
-      <c r="BY6" s="79" t="str">
+      <c r="BY6" s="65" t="str">
         <f t="shared" si="26"/>
         <v/>
       </c>
-      <c r="BZ6" s="79"/>
+      <c r="BZ6" s="65"/>
       <c r="CA6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CB6" s="1"/>
-      <c r="CC6" s="78" t="str">
+      <c r="CC6" s="66" t="str">
         <f t="shared" si="16"/>
         <v/>
       </c>
-      <c r="CD6" s="78"/>
+      <c r="CD6" s="66"/>
       <c r="CE6" s="6"/>
       <c r="CF6" s="1"/>
       <c r="CG6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="CH6" s="1"/>
-      <c r="CI6" s="79" t="str">
+      <c r="CI6" s="65" t="str">
         <f t="shared" si="27"/>
         <v/>
       </c>
-      <c r="CJ6" s="79"/>
+      <c r="CJ6" s="65"/>
       <c r="CK6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CL6" s="1"/>
-      <c r="CM6" s="78" t="str">
+      <c r="CM6" s="66" t="str">
         <f t="shared" si="17"/>
         <v/>
       </c>
-      <c r="CN6" s="78"/>
+      <c r="CN6" s="66"/>
       <c r="CO6" s="6"/>
       <c r="CP6" s="1"/>
       <c r="CQ6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="CR6" s="1"/>
-      <c r="CS6" s="79" t="str">
+      <c r="CS6" s="65" t="str">
         <f t="shared" si="28"/>
         <v/>
       </c>
-      <c r="CT6" s="79"/>
+      <c r="CT6" s="65"/>
       <c r="CU6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="CV6" s="1"/>
-      <c r="CW6" s="78" t="str">
+      <c r="CW6" s="66" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="CX6" s="78"/>
+      <c r="CX6" s="66"/>
       <c r="CY6" s="6"/>
       <c r="CZ6" s="1"/>
       <c r="DA6" s="1" t="s">
         <v>2</v>
       </c>
       <c r="DB6" s="1"/>
-      <c r="DC6" s="79" t="str">
+      <c r="DC6" s="65" t="str">
         <f t="shared" si="29"/>
         <v/>
       </c>
-      <c r="DD6" s="79"/>
+      <c r="DD6" s="65"/>
       <c r="DE6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="DF6" s="1"/>
-      <c r="DG6" s="78" t="str">
+      <c r="DG6" s="66" t="str">
         <f t="shared" si="19"/>
         <v/>
       </c>
-      <c r="DH6" s="78"/>
+      <c r="DH6" s="66"/>
       <c r="DI6" s="6"/>
     </row>
     <row r="7" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5555,11 +5555,11 @@
       <c r="DI32" s="29"/>
     </row>
     <row r="33" spans="1:113" s="19" customFormat="1" ht="119.65" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
       <c r="D33" s="29"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
@@ -6588,116 +6588,146 @@
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="82"/>
-      <c r="G42" s="82"/>
-      <c r="H42" s="82"/>
-      <c r="I42" s="82"/>
-      <c r="J42" s="82"/>
-      <c r="K42" s="82"/>
-      <c r="L42" s="82"/>
-      <c r="M42" s="82"/>
-      <c r="N42" s="82"/>
-      <c r="O42" s="82"/>
-      <c r="P42" s="82"/>
-      <c r="Q42" s="82"/>
-      <c r="R42" s="82"/>
-      <c r="S42" s="82"/>
-      <c r="T42" s="82"/>
-      <c r="U42" s="82"/>
-      <c r="V42" s="82"/>
-      <c r="W42" s="82"/>
-      <c r="X42" s="82"/>
-      <c r="Y42" s="82"/>
-      <c r="Z42" s="82"/>
-      <c r="AA42" s="82"/>
-      <c r="AB42" s="82"/>
-      <c r="AC42" s="82"/>
-      <c r="AD42" s="82"/>
-      <c r="AE42" s="82"/>
-      <c r="AF42" s="82"/>
-      <c r="AG42" s="82"/>
-      <c r="AH42" s="82"/>
-      <c r="AI42" s="82"/>
-      <c r="AJ42" s="82"/>
-      <c r="AK42" s="82"/>
-      <c r="AL42" s="82"/>
-      <c r="AM42" s="82"/>
-      <c r="AN42" s="82"/>
-      <c r="AO42" s="82"/>
-      <c r="AP42" s="82"/>
-      <c r="AQ42" s="82"/>
-      <c r="AR42" s="82"/>
-      <c r="AS42" s="82"/>
-      <c r="AT42" s="82"/>
-      <c r="AU42" s="82"/>
-      <c r="AV42" s="82"/>
-      <c r="AW42" s="82"/>
-      <c r="AX42" s="82"/>
-      <c r="AY42" s="82"/>
-      <c r="AZ42" s="82"/>
-      <c r="BA42" s="82"/>
-      <c r="BB42" s="82"/>
-      <c r="BC42" s="82"/>
-      <c r="BD42" s="82"/>
-      <c r="BE42" s="82"/>
-      <c r="BF42" s="82"/>
-      <c r="BG42" s="82"/>
-      <c r="BH42" s="82"/>
-      <c r="BI42" s="82"/>
-      <c r="BJ42" s="82"/>
-      <c r="BK42" s="82"/>
-      <c r="BL42" s="82"/>
-      <c r="BM42" s="82"/>
-      <c r="BN42" s="82"/>
-      <c r="BO42" s="82"/>
-      <c r="BP42" s="82"/>
-      <c r="BQ42" s="82"/>
-      <c r="BR42" s="82"/>
-      <c r="BS42" s="82"/>
-      <c r="BT42" s="82"/>
-      <c r="BU42" s="82"/>
-      <c r="BV42" s="82"/>
-      <c r="BW42" s="82"/>
-      <c r="BX42" s="82"/>
-      <c r="BY42" s="82"/>
-      <c r="BZ42" s="82"/>
-      <c r="CA42" s="82"/>
-      <c r="CB42" s="82"/>
-      <c r="CC42" s="82"/>
-      <c r="CD42" s="82"/>
-      <c r="CE42" s="82"/>
-      <c r="CF42" s="82"/>
-      <c r="CG42" s="82"/>
-      <c r="CH42" s="82"/>
-      <c r="CI42" s="82"/>
-      <c r="CJ42" s="82"/>
-      <c r="CK42" s="82"/>
-      <c r="CL42" s="82"/>
-      <c r="CM42" s="82"/>
-      <c r="CN42" s="82"/>
-      <c r="CO42" s="82"/>
-      <c r="CP42" s="82"/>
-      <c r="CQ42" s="82"/>
-      <c r="CR42" s="82"/>
-      <c r="CS42" s="82"/>
-      <c r="CT42" s="82"/>
-      <c r="CU42" s="82"/>
-      <c r="CV42" s="82"/>
-      <c r="CW42" s="82"/>
-      <c r="CX42" s="82"/>
-      <c r="CY42" s="82"/>
-      <c r="CZ42" s="82"/>
-      <c r="DA42" s="82"/>
-      <c r="DB42" s="82"/>
-      <c r="DC42" s="82"/>
-      <c r="DD42" s="82"/>
-      <c r="DE42" s="82"/>
-      <c r="DF42" s="82"/>
-      <c r="DG42" s="82"/>
-      <c r="DH42" s="82"/>
-      <c r="DI42" s="82"/>
+      <c r="D42" s="64"/>
+      <c r="E42" s="64"/>
+      <c r="F42" s="64"/>
+      <c r="G42" s="64"/>
+      <c r="H42" s="64"/>
+      <c r="I42" s="64"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="64"/>
+      <c r="N42" s="64" t="str">
+        <f>IF(ISBLANK(D42),"",D42)</f>
+        <v/>
+      </c>
+      <c r="O42" s="64"/>
+      <c r="P42" s="64"/>
+      <c r="Q42" s="64"/>
+      <c r="R42" s="64"/>
+      <c r="S42" s="64"/>
+      <c r="T42" s="64"/>
+      <c r="U42" s="64"/>
+      <c r="V42" s="64"/>
+      <c r="W42" s="64"/>
+      <c r="X42" s="64" t="str">
+        <f t="shared" ref="X42" si="33">IF(ISBLANK(N42),"",N42)</f>
+        <v/>
+      </c>
+      <c r="Y42" s="64"/>
+      <c r="Z42" s="64"/>
+      <c r="AA42" s="64"/>
+      <c r="AB42" s="64"/>
+      <c r="AC42" s="64"/>
+      <c r="AD42" s="64"/>
+      <c r="AE42" s="64"/>
+      <c r="AF42" s="64"/>
+      <c r="AG42" s="64"/>
+      <c r="AH42" s="64" t="str">
+        <f t="shared" ref="AH42" si="34">IF(ISBLANK(X42),"",X42)</f>
+        <v/>
+      </c>
+      <c r="AI42" s="64"/>
+      <c r="AJ42" s="64"/>
+      <c r="AK42" s="64"/>
+      <c r="AL42" s="64"/>
+      <c r="AM42" s="64"/>
+      <c r="AN42" s="64"/>
+      <c r="AO42" s="64"/>
+      <c r="AP42" s="64"/>
+      <c r="AQ42" s="64"/>
+      <c r="AR42" s="64" t="str">
+        <f t="shared" ref="AR42" si="35">IF(ISBLANK(AH42),"",AH42)</f>
+        <v/>
+      </c>
+      <c r="AS42" s="64"/>
+      <c r="AT42" s="64"/>
+      <c r="AU42" s="64"/>
+      <c r="AV42" s="64"/>
+      <c r="AW42" s="64"/>
+      <c r="AX42" s="64"/>
+      <c r="AY42" s="64"/>
+      <c r="AZ42" s="64"/>
+      <c r="BA42" s="64"/>
+      <c r="BB42" s="64" t="str">
+        <f t="shared" ref="BB42" si="36">IF(ISBLANK(AR42),"",AR42)</f>
+        <v/>
+      </c>
+      <c r="BC42" s="64"/>
+      <c r="BD42" s="64"/>
+      <c r="BE42" s="64"/>
+      <c r="BF42" s="64"/>
+      <c r="BG42" s="64"/>
+      <c r="BH42" s="64"/>
+      <c r="BI42" s="64"/>
+      <c r="BJ42" s="64"/>
+      <c r="BK42" s="64"/>
+      <c r="BL42" s="64" t="str">
+        <f t="shared" ref="BL42" si="37">IF(ISBLANK(BB42),"",BB42)</f>
+        <v/>
+      </c>
+      <c r="BM42" s="64"/>
+      <c r="BN42" s="64"/>
+      <c r="BO42" s="64"/>
+      <c r="BP42" s="64"/>
+      <c r="BQ42" s="64"/>
+      <c r="BR42" s="64"/>
+      <c r="BS42" s="64"/>
+      <c r="BT42" s="64"/>
+      <c r="BU42" s="64"/>
+      <c r="BV42" s="64" t="str">
+        <f t="shared" ref="BV42" si="38">IF(ISBLANK(BL42),"",BL42)</f>
+        <v/>
+      </c>
+      <c r="BW42" s="64"/>
+      <c r="BX42" s="64"/>
+      <c r="BY42" s="64"/>
+      <c r="BZ42" s="64"/>
+      <c r="CA42" s="64"/>
+      <c r="CB42" s="64"/>
+      <c r="CC42" s="64"/>
+      <c r="CD42" s="64"/>
+      <c r="CE42" s="64"/>
+      <c r="CF42" s="64" t="str">
+        <f t="shared" ref="CF42" si="39">IF(ISBLANK(BV42),"",BV42)</f>
+        <v/>
+      </c>
+      <c r="CG42" s="64"/>
+      <c r="CH42" s="64"/>
+      <c r="CI42" s="64"/>
+      <c r="CJ42" s="64"/>
+      <c r="CK42" s="64"/>
+      <c r="CL42" s="64"/>
+      <c r="CM42" s="64"/>
+      <c r="CN42" s="64"/>
+      <c r="CO42" s="64"/>
+      <c r="CP42" s="64" t="str">
+        <f t="shared" ref="CP42" si="40">IF(ISBLANK(CF42),"",CF42)</f>
+        <v/>
+      </c>
+      <c r="CQ42" s="64"/>
+      <c r="CR42" s="64"/>
+      <c r="CS42" s="64"/>
+      <c r="CT42" s="64"/>
+      <c r="CU42" s="64"/>
+      <c r="CV42" s="64"/>
+      <c r="CW42" s="64"/>
+      <c r="CX42" s="64"/>
+      <c r="CY42" s="64"/>
+      <c r="CZ42" s="64" t="str">
+        <f>IF(ISBLANK(CP42),"",CP42)</f>
+        <v/>
+      </c>
+      <c r="DA42" s="64"/>
+      <c r="DB42" s="64"/>
+      <c r="DC42" s="64"/>
+      <c r="DD42" s="64"/>
+      <c r="DE42" s="64"/>
+      <c r="DF42" s="64"/>
+      <c r="DG42" s="64"/>
+      <c r="DH42" s="64"/>
+      <c r="DI42" s="64"/>
     </row>
     <row r="43" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
@@ -6705,461 +6735,461 @@
         <v>51</v>
       </c>
       <c r="C43" s="1"/>
-      <c r="D43" s="82"/>
-      <c r="E43" s="82"/>
-      <c r="F43" s="82"/>
-      <c r="G43" s="82"/>
-      <c r="H43" s="82"/>
-      <c r="I43" s="82"/>
-      <c r="J43" s="82"/>
-      <c r="K43" s="82"/>
-      <c r="L43" s="82"/>
-      <c r="M43" s="82"/>
-      <c r="N43" s="82"/>
-      <c r="O43" s="82"/>
-      <c r="P43" s="82"/>
-      <c r="Q43" s="82"/>
-      <c r="R43" s="82"/>
-      <c r="S43" s="82"/>
-      <c r="T43" s="82"/>
-      <c r="U43" s="82"/>
-      <c r="V43" s="82"/>
-      <c r="W43" s="82"/>
-      <c r="X43" s="82"/>
-      <c r="Y43" s="82"/>
-      <c r="Z43" s="82"/>
-      <c r="AA43" s="82"/>
-      <c r="AB43" s="82"/>
-      <c r="AC43" s="82"/>
-      <c r="AD43" s="82"/>
-      <c r="AE43" s="82"/>
-      <c r="AF43" s="82"/>
-      <c r="AG43" s="82"/>
-      <c r="AH43" s="82"/>
-      <c r="AI43" s="82"/>
-      <c r="AJ43" s="82"/>
-      <c r="AK43" s="82"/>
-      <c r="AL43" s="82"/>
-      <c r="AM43" s="82"/>
-      <c r="AN43" s="82"/>
-      <c r="AO43" s="82"/>
-      <c r="AP43" s="82"/>
-      <c r="AQ43" s="82"/>
-      <c r="AR43" s="82"/>
-      <c r="AS43" s="82"/>
-      <c r="AT43" s="82"/>
-      <c r="AU43" s="82"/>
-      <c r="AV43" s="82"/>
-      <c r="AW43" s="82"/>
-      <c r="AX43" s="82"/>
-      <c r="AY43" s="82"/>
-      <c r="AZ43" s="82"/>
-      <c r="BA43" s="82"/>
-      <c r="BB43" s="82"/>
-      <c r="BC43" s="82"/>
-      <c r="BD43" s="82"/>
-      <c r="BE43" s="82"/>
-      <c r="BF43" s="82"/>
-      <c r="BG43" s="82"/>
-      <c r="BH43" s="82"/>
-      <c r="BI43" s="82"/>
-      <c r="BJ43" s="82"/>
-      <c r="BK43" s="82"/>
-      <c r="BL43" s="82"/>
-      <c r="BM43" s="82"/>
-      <c r="BN43" s="82"/>
-      <c r="BO43" s="82"/>
-      <c r="BP43" s="82"/>
-      <c r="BQ43" s="82"/>
-      <c r="BR43" s="82"/>
-      <c r="BS43" s="82"/>
-      <c r="BT43" s="82"/>
-      <c r="BU43" s="82"/>
-      <c r="BV43" s="82"/>
-      <c r="BW43" s="82"/>
-      <c r="BX43" s="82"/>
-      <c r="BY43" s="82"/>
-      <c r="BZ43" s="82"/>
-      <c r="CA43" s="82"/>
-      <c r="CB43" s="82"/>
-      <c r="CC43" s="82"/>
-      <c r="CD43" s="82"/>
-      <c r="CE43" s="82"/>
-      <c r="CF43" s="82"/>
-      <c r="CG43" s="82"/>
-      <c r="CH43" s="82"/>
-      <c r="CI43" s="82"/>
-      <c r="CJ43" s="82"/>
-      <c r="CK43" s="82"/>
-      <c r="CL43" s="82"/>
-      <c r="CM43" s="82"/>
-      <c r="CN43" s="82"/>
-      <c r="CO43" s="82"/>
-      <c r="CP43" s="82"/>
-      <c r="CQ43" s="82"/>
-      <c r="CR43" s="82"/>
-      <c r="CS43" s="82"/>
-      <c r="CT43" s="82"/>
-      <c r="CU43" s="82"/>
-      <c r="CV43" s="82"/>
-      <c r="CW43" s="82"/>
-      <c r="CX43" s="82"/>
-      <c r="CY43" s="82"/>
-      <c r="CZ43" s="82"/>
-      <c r="DA43" s="82"/>
-      <c r="DB43" s="82"/>
-      <c r="DC43" s="82"/>
-      <c r="DD43" s="82"/>
-      <c r="DE43" s="82"/>
-      <c r="DF43" s="82"/>
-      <c r="DG43" s="82"/>
-      <c r="DH43" s="82"/>
-      <c r="DI43" s="82"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="64"/>
+      <c r="H43" s="64"/>
+      <c r="I43" s="64"/>
+      <c r="J43" s="64"/>
+      <c r="K43" s="64"/>
+      <c r="L43" s="64"/>
+      <c r="M43" s="64"/>
+      <c r="N43" s="64"/>
+      <c r="O43" s="64"/>
+      <c r="P43" s="64"/>
+      <c r="Q43" s="64"/>
+      <c r="R43" s="64"/>
+      <c r="S43" s="64"/>
+      <c r="T43" s="64"/>
+      <c r="U43" s="64"/>
+      <c r="V43" s="64"/>
+      <c r="W43" s="64"/>
+      <c r="X43" s="64"/>
+      <c r="Y43" s="64"/>
+      <c r="Z43" s="64"/>
+      <c r="AA43" s="64"/>
+      <c r="AB43" s="64"/>
+      <c r="AC43" s="64"/>
+      <c r="AD43" s="64"/>
+      <c r="AE43" s="64"/>
+      <c r="AF43" s="64"/>
+      <c r="AG43" s="64"/>
+      <c r="AH43" s="64"/>
+      <c r="AI43" s="64"/>
+      <c r="AJ43" s="64"/>
+      <c r="AK43" s="64"/>
+      <c r="AL43" s="64"/>
+      <c r="AM43" s="64"/>
+      <c r="AN43" s="64"/>
+      <c r="AO43" s="64"/>
+      <c r="AP43" s="64"/>
+      <c r="AQ43" s="64"/>
+      <c r="AR43" s="64"/>
+      <c r="AS43" s="64"/>
+      <c r="AT43" s="64"/>
+      <c r="AU43" s="64"/>
+      <c r="AV43" s="64"/>
+      <c r="AW43" s="64"/>
+      <c r="AX43" s="64"/>
+      <c r="AY43" s="64"/>
+      <c r="AZ43" s="64"/>
+      <c r="BA43" s="64"/>
+      <c r="BB43" s="64"/>
+      <c r="BC43" s="64"/>
+      <c r="BD43" s="64"/>
+      <c r="BE43" s="64"/>
+      <c r="BF43" s="64"/>
+      <c r="BG43" s="64"/>
+      <c r="BH43" s="64"/>
+      <c r="BI43" s="64"/>
+      <c r="BJ43" s="64"/>
+      <c r="BK43" s="64"/>
+      <c r="BL43" s="64"/>
+      <c r="BM43" s="64"/>
+      <c r="BN43" s="64"/>
+      <c r="BO43" s="64"/>
+      <c r="BP43" s="64"/>
+      <c r="BQ43" s="64"/>
+      <c r="BR43" s="64"/>
+      <c r="BS43" s="64"/>
+      <c r="BT43" s="64"/>
+      <c r="BU43" s="64"/>
+      <c r="BV43" s="64"/>
+      <c r="BW43" s="64"/>
+      <c r="BX43" s="64"/>
+      <c r="BY43" s="64"/>
+      <c r="BZ43" s="64"/>
+      <c r="CA43" s="64"/>
+      <c r="CB43" s="64"/>
+      <c r="CC43" s="64"/>
+      <c r="CD43" s="64"/>
+      <c r="CE43" s="64"/>
+      <c r="CF43" s="64"/>
+      <c r="CG43" s="64"/>
+      <c r="CH43" s="64"/>
+      <c r="CI43" s="64"/>
+      <c r="CJ43" s="64"/>
+      <c r="CK43" s="64"/>
+      <c r="CL43" s="64"/>
+      <c r="CM43" s="64"/>
+      <c r="CN43" s="64"/>
+      <c r="CO43" s="64"/>
+      <c r="CP43" s="64"/>
+      <c r="CQ43" s="64"/>
+      <c r="CR43" s="64"/>
+      <c r="CS43" s="64"/>
+      <c r="CT43" s="64"/>
+      <c r="CU43" s="64"/>
+      <c r="CV43" s="64"/>
+      <c r="CW43" s="64"/>
+      <c r="CX43" s="64"/>
+      <c r="CY43" s="64"/>
+      <c r="CZ43" s="64"/>
+      <c r="DA43" s="64"/>
+      <c r="DB43" s="64"/>
+      <c r="DC43" s="64"/>
+      <c r="DD43" s="64"/>
+      <c r="DE43" s="64"/>
+      <c r="DF43" s="64"/>
+      <c r="DG43" s="64"/>
+      <c r="DH43" s="64"/>
+      <c r="DI43" s="64"/>
     </row>
     <row r="44" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="82"/>
-      <c r="H44" s="82"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="82"/>
-      <c r="K44" s="82"/>
-      <c r="L44" s="82"/>
-      <c r="M44" s="82"/>
-      <c r="N44" s="82"/>
-      <c r="O44" s="82"/>
-      <c r="P44" s="82"/>
-      <c r="Q44" s="82"/>
-      <c r="R44" s="82"/>
-      <c r="S44" s="82"/>
-      <c r="T44" s="82"/>
-      <c r="U44" s="82"/>
-      <c r="V44" s="82"/>
-      <c r="W44" s="82"/>
-      <c r="X44" s="82"/>
-      <c r="Y44" s="82"/>
-      <c r="Z44" s="82"/>
-      <c r="AA44" s="82"/>
-      <c r="AB44" s="82"/>
-      <c r="AC44" s="82"/>
-      <c r="AD44" s="82"/>
-      <c r="AE44" s="82"/>
-      <c r="AF44" s="82"/>
-      <c r="AG44" s="82"/>
-      <c r="AH44" s="82"/>
-      <c r="AI44" s="82"/>
-      <c r="AJ44" s="82"/>
-      <c r="AK44" s="82"/>
-      <c r="AL44" s="82"/>
-      <c r="AM44" s="82"/>
-      <c r="AN44" s="82"/>
-      <c r="AO44" s="82"/>
-      <c r="AP44" s="82"/>
-      <c r="AQ44" s="82"/>
-      <c r="AR44" s="82"/>
-      <c r="AS44" s="82"/>
-      <c r="AT44" s="82"/>
-      <c r="AU44" s="82"/>
-      <c r="AV44" s="82"/>
-      <c r="AW44" s="82"/>
-      <c r="AX44" s="82"/>
-      <c r="AY44" s="82"/>
-      <c r="AZ44" s="82"/>
-      <c r="BA44" s="82"/>
-      <c r="BB44" s="82"/>
-      <c r="BC44" s="82"/>
-      <c r="BD44" s="82"/>
-      <c r="BE44" s="82"/>
-      <c r="BF44" s="82"/>
-      <c r="BG44" s="82"/>
-      <c r="BH44" s="82"/>
-      <c r="BI44" s="82"/>
-      <c r="BJ44" s="82"/>
-      <c r="BK44" s="82"/>
-      <c r="BL44" s="82"/>
-      <c r="BM44" s="82"/>
-      <c r="BN44" s="82"/>
-      <c r="BO44" s="82"/>
-      <c r="BP44" s="82"/>
-      <c r="BQ44" s="82"/>
-      <c r="BR44" s="82"/>
-      <c r="BS44" s="82"/>
-      <c r="BT44" s="82"/>
-      <c r="BU44" s="82"/>
-      <c r="BV44" s="82"/>
-      <c r="BW44" s="82"/>
-      <c r="BX44" s="82"/>
-      <c r="BY44" s="82"/>
-      <c r="BZ44" s="82"/>
-      <c r="CA44" s="82"/>
-      <c r="CB44" s="82"/>
-      <c r="CC44" s="82"/>
-      <c r="CD44" s="82"/>
-      <c r="CE44" s="82"/>
-      <c r="CF44" s="82"/>
-      <c r="CG44" s="82"/>
-      <c r="CH44" s="82"/>
-      <c r="CI44" s="82"/>
-      <c r="CJ44" s="82"/>
-      <c r="CK44" s="82"/>
-      <c r="CL44" s="82"/>
-      <c r="CM44" s="82"/>
-      <c r="CN44" s="82"/>
-      <c r="CO44" s="82"/>
-      <c r="CP44" s="82"/>
-      <c r="CQ44" s="82"/>
-      <c r="CR44" s="82"/>
-      <c r="CS44" s="82"/>
-      <c r="CT44" s="82"/>
-      <c r="CU44" s="82"/>
-      <c r="CV44" s="82"/>
-      <c r="CW44" s="82"/>
-      <c r="CX44" s="82"/>
-      <c r="CY44" s="82"/>
-      <c r="CZ44" s="82"/>
-      <c r="DA44" s="82"/>
-      <c r="DB44" s="82"/>
-      <c r="DC44" s="82"/>
-      <c r="DD44" s="82"/>
-      <c r="DE44" s="82"/>
-      <c r="DF44" s="82"/>
-      <c r="DG44" s="82"/>
-      <c r="DH44" s="82"/>
-      <c r="DI44" s="82"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="64"/>
+      <c r="H44" s="64"/>
+      <c r="I44" s="64"/>
+      <c r="J44" s="64"/>
+      <c r="K44" s="64"/>
+      <c r="L44" s="64"/>
+      <c r="M44" s="64"/>
+      <c r="N44" s="64"/>
+      <c r="O44" s="64"/>
+      <c r="P44" s="64"/>
+      <c r="Q44" s="64"/>
+      <c r="R44" s="64"/>
+      <c r="S44" s="64"/>
+      <c r="T44" s="64"/>
+      <c r="U44" s="64"/>
+      <c r="V44" s="64"/>
+      <c r="W44" s="64"/>
+      <c r="X44" s="64"/>
+      <c r="Y44" s="64"/>
+      <c r="Z44" s="64"/>
+      <c r="AA44" s="64"/>
+      <c r="AB44" s="64"/>
+      <c r="AC44" s="64"/>
+      <c r="AD44" s="64"/>
+      <c r="AE44" s="64"/>
+      <c r="AF44" s="64"/>
+      <c r="AG44" s="64"/>
+      <c r="AH44" s="64"/>
+      <c r="AI44" s="64"/>
+      <c r="AJ44" s="64"/>
+      <c r="AK44" s="64"/>
+      <c r="AL44" s="64"/>
+      <c r="AM44" s="64"/>
+      <c r="AN44" s="64"/>
+      <c r="AO44" s="64"/>
+      <c r="AP44" s="64"/>
+      <c r="AQ44" s="64"/>
+      <c r="AR44" s="64"/>
+      <c r="AS44" s="64"/>
+      <c r="AT44" s="64"/>
+      <c r="AU44" s="64"/>
+      <c r="AV44" s="64"/>
+      <c r="AW44" s="64"/>
+      <c r="AX44" s="64"/>
+      <c r="AY44" s="64"/>
+      <c r="AZ44" s="64"/>
+      <c r="BA44" s="64"/>
+      <c r="BB44" s="64"/>
+      <c r="BC44" s="64"/>
+      <c r="BD44" s="64"/>
+      <c r="BE44" s="64"/>
+      <c r="BF44" s="64"/>
+      <c r="BG44" s="64"/>
+      <c r="BH44" s="64"/>
+      <c r="BI44" s="64"/>
+      <c r="BJ44" s="64"/>
+      <c r="BK44" s="64"/>
+      <c r="BL44" s="64"/>
+      <c r="BM44" s="64"/>
+      <c r="BN44" s="64"/>
+      <c r="BO44" s="64"/>
+      <c r="BP44" s="64"/>
+      <c r="BQ44" s="64"/>
+      <c r="BR44" s="64"/>
+      <c r="BS44" s="64"/>
+      <c r="BT44" s="64"/>
+      <c r="BU44" s="64"/>
+      <c r="BV44" s="64"/>
+      <c r="BW44" s="64"/>
+      <c r="BX44" s="64"/>
+      <c r="BY44" s="64"/>
+      <c r="BZ44" s="64"/>
+      <c r="CA44" s="64"/>
+      <c r="CB44" s="64"/>
+      <c r="CC44" s="64"/>
+      <c r="CD44" s="64"/>
+      <c r="CE44" s="64"/>
+      <c r="CF44" s="64"/>
+      <c r="CG44" s="64"/>
+      <c r="CH44" s="64"/>
+      <c r="CI44" s="64"/>
+      <c r="CJ44" s="64"/>
+      <c r="CK44" s="64"/>
+      <c r="CL44" s="64"/>
+      <c r="CM44" s="64"/>
+      <c r="CN44" s="64"/>
+      <c r="CO44" s="64"/>
+      <c r="CP44" s="64"/>
+      <c r="CQ44" s="64"/>
+      <c r="CR44" s="64"/>
+      <c r="CS44" s="64"/>
+      <c r="CT44" s="64"/>
+      <c r="CU44" s="64"/>
+      <c r="CV44" s="64"/>
+      <c r="CW44" s="64"/>
+      <c r="CX44" s="64"/>
+      <c r="CY44" s="64"/>
+      <c r="CZ44" s="64"/>
+      <c r="DA44" s="64"/>
+      <c r="DB44" s="64"/>
+      <c r="DC44" s="64"/>
+      <c r="DD44" s="64"/>
+      <c r="DE44" s="64"/>
+      <c r="DF44" s="64"/>
+      <c r="DG44" s="64"/>
+      <c r="DH44" s="64"/>
+      <c r="DI44" s="64"/>
     </row>
     <row r="45" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
-      <c r="D45" s="82"/>
-      <c r="E45" s="82"/>
-      <c r="F45" s="82"/>
-      <c r="G45" s="82"/>
-      <c r="H45" s="82"/>
-      <c r="I45" s="82"/>
-      <c r="J45" s="82"/>
-      <c r="K45" s="82"/>
-      <c r="L45" s="82"/>
-      <c r="M45" s="82"/>
-      <c r="N45" s="82"/>
-      <c r="O45" s="82"/>
-      <c r="P45" s="82"/>
-      <c r="Q45" s="82"/>
-      <c r="R45" s="82"/>
-      <c r="S45" s="82"/>
-      <c r="T45" s="82"/>
-      <c r="U45" s="82"/>
-      <c r="V45" s="82"/>
-      <c r="W45" s="82"/>
-      <c r="X45" s="82"/>
-      <c r="Y45" s="82"/>
-      <c r="Z45" s="82"/>
-      <c r="AA45" s="82"/>
-      <c r="AB45" s="82"/>
-      <c r="AC45" s="82"/>
-      <c r="AD45" s="82"/>
-      <c r="AE45" s="82"/>
-      <c r="AF45" s="82"/>
-      <c r="AG45" s="82"/>
-      <c r="AH45" s="82"/>
-      <c r="AI45" s="82"/>
-      <c r="AJ45" s="82"/>
-      <c r="AK45" s="82"/>
-      <c r="AL45" s="82"/>
-      <c r="AM45" s="82"/>
-      <c r="AN45" s="82"/>
-      <c r="AO45" s="82"/>
-      <c r="AP45" s="82"/>
-      <c r="AQ45" s="82"/>
-      <c r="AR45" s="82"/>
-      <c r="AS45" s="82"/>
-      <c r="AT45" s="82"/>
-      <c r="AU45" s="82"/>
-      <c r="AV45" s="82"/>
-      <c r="AW45" s="82"/>
-      <c r="AX45" s="82"/>
-      <c r="AY45" s="82"/>
-      <c r="AZ45" s="82"/>
-      <c r="BA45" s="82"/>
-      <c r="BB45" s="82"/>
-      <c r="BC45" s="82"/>
-      <c r="BD45" s="82"/>
-      <c r="BE45" s="82"/>
-      <c r="BF45" s="82"/>
-      <c r="BG45" s="82"/>
-      <c r="BH45" s="82"/>
-      <c r="BI45" s="82"/>
-      <c r="BJ45" s="82"/>
-      <c r="BK45" s="82"/>
-      <c r="BL45" s="82"/>
-      <c r="BM45" s="82"/>
-      <c r="BN45" s="82"/>
-      <c r="BO45" s="82"/>
-      <c r="BP45" s="82"/>
-      <c r="BQ45" s="82"/>
-      <c r="BR45" s="82"/>
-      <c r="BS45" s="82"/>
-      <c r="BT45" s="82"/>
-      <c r="BU45" s="82"/>
-      <c r="BV45" s="82"/>
-      <c r="BW45" s="82"/>
-      <c r="BX45" s="82"/>
-      <c r="BY45" s="82"/>
-      <c r="BZ45" s="82"/>
-      <c r="CA45" s="82"/>
-      <c r="CB45" s="82"/>
-      <c r="CC45" s="82"/>
-      <c r="CD45" s="82"/>
-      <c r="CE45" s="82"/>
-      <c r="CF45" s="82"/>
-      <c r="CG45" s="82"/>
-      <c r="CH45" s="82"/>
-      <c r="CI45" s="82"/>
-      <c r="CJ45" s="82"/>
-      <c r="CK45" s="82"/>
-      <c r="CL45" s="82"/>
-      <c r="CM45" s="82"/>
-      <c r="CN45" s="82"/>
-      <c r="CO45" s="82"/>
-      <c r="CP45" s="82"/>
-      <c r="CQ45" s="82"/>
-      <c r="CR45" s="82"/>
-      <c r="CS45" s="82"/>
-      <c r="CT45" s="82"/>
-      <c r="CU45" s="82"/>
-      <c r="CV45" s="82"/>
-      <c r="CW45" s="82"/>
-      <c r="CX45" s="82"/>
-      <c r="CY45" s="82"/>
-      <c r="CZ45" s="82"/>
-      <c r="DA45" s="82"/>
-      <c r="DB45" s="82"/>
-      <c r="DC45" s="82"/>
-      <c r="DD45" s="82"/>
-      <c r="DE45" s="82"/>
-      <c r="DF45" s="82"/>
-      <c r="DG45" s="82"/>
-      <c r="DH45" s="82"/>
-      <c r="DI45" s="82"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="64"/>
+      <c r="I45" s="64"/>
+      <c r="J45" s="64"/>
+      <c r="K45" s="64"/>
+      <c r="L45" s="64"/>
+      <c r="M45" s="64"/>
+      <c r="N45" s="64"/>
+      <c r="O45" s="64"/>
+      <c r="P45" s="64"/>
+      <c r="Q45" s="64"/>
+      <c r="R45" s="64"/>
+      <c r="S45" s="64"/>
+      <c r="T45" s="64"/>
+      <c r="U45" s="64"/>
+      <c r="V45" s="64"/>
+      <c r="W45" s="64"/>
+      <c r="X45" s="64"/>
+      <c r="Y45" s="64"/>
+      <c r="Z45" s="64"/>
+      <c r="AA45" s="64"/>
+      <c r="AB45" s="64"/>
+      <c r="AC45" s="64"/>
+      <c r="AD45" s="64"/>
+      <c r="AE45" s="64"/>
+      <c r="AF45" s="64"/>
+      <c r="AG45" s="64"/>
+      <c r="AH45" s="64"/>
+      <c r="AI45" s="64"/>
+      <c r="AJ45" s="64"/>
+      <c r="AK45" s="64"/>
+      <c r="AL45" s="64"/>
+      <c r="AM45" s="64"/>
+      <c r="AN45" s="64"/>
+      <c r="AO45" s="64"/>
+      <c r="AP45" s="64"/>
+      <c r="AQ45" s="64"/>
+      <c r="AR45" s="64"/>
+      <c r="AS45" s="64"/>
+      <c r="AT45" s="64"/>
+      <c r="AU45" s="64"/>
+      <c r="AV45" s="64"/>
+      <c r="AW45" s="64"/>
+      <c r="AX45" s="64"/>
+      <c r="AY45" s="64"/>
+      <c r="AZ45" s="64"/>
+      <c r="BA45" s="64"/>
+      <c r="BB45" s="64"/>
+      <c r="BC45" s="64"/>
+      <c r="BD45" s="64"/>
+      <c r="BE45" s="64"/>
+      <c r="BF45" s="64"/>
+      <c r="BG45" s="64"/>
+      <c r="BH45" s="64"/>
+      <c r="BI45" s="64"/>
+      <c r="BJ45" s="64"/>
+      <c r="BK45" s="64"/>
+      <c r="BL45" s="64"/>
+      <c r="BM45" s="64"/>
+      <c r="BN45" s="64"/>
+      <c r="BO45" s="64"/>
+      <c r="BP45" s="64"/>
+      <c r="BQ45" s="64"/>
+      <c r="BR45" s="64"/>
+      <c r="BS45" s="64"/>
+      <c r="BT45" s="64"/>
+      <c r="BU45" s="64"/>
+      <c r="BV45" s="64"/>
+      <c r="BW45" s="64"/>
+      <c r="BX45" s="64"/>
+      <c r="BY45" s="64"/>
+      <c r="BZ45" s="64"/>
+      <c r="CA45" s="64"/>
+      <c r="CB45" s="64"/>
+      <c r="CC45" s="64"/>
+      <c r="CD45" s="64"/>
+      <c r="CE45" s="64"/>
+      <c r="CF45" s="64"/>
+      <c r="CG45" s="64"/>
+      <c r="CH45" s="64"/>
+      <c r="CI45" s="64"/>
+      <c r="CJ45" s="64"/>
+      <c r="CK45" s="64"/>
+      <c r="CL45" s="64"/>
+      <c r="CM45" s="64"/>
+      <c r="CN45" s="64"/>
+      <c r="CO45" s="64"/>
+      <c r="CP45" s="64"/>
+      <c r="CQ45" s="64"/>
+      <c r="CR45" s="64"/>
+      <c r="CS45" s="64"/>
+      <c r="CT45" s="64"/>
+      <c r="CU45" s="64"/>
+      <c r="CV45" s="64"/>
+      <c r="CW45" s="64"/>
+      <c r="CX45" s="64"/>
+      <c r="CY45" s="64"/>
+      <c r="CZ45" s="64"/>
+      <c r="DA45" s="64"/>
+      <c r="DB45" s="64"/>
+      <c r="DC45" s="64"/>
+      <c r="DD45" s="64"/>
+      <c r="DE45" s="64"/>
+      <c r="DF45" s="64"/>
+      <c r="DG45" s="64"/>
+      <c r="DH45" s="64"/>
+      <c r="DI45" s="64"/>
     </row>
     <row r="46" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
-      <c r="D46" s="82"/>
-      <c r="E46" s="82"/>
-      <c r="F46" s="82"/>
-      <c r="G46" s="82"/>
-      <c r="H46" s="82"/>
-      <c r="I46" s="82"/>
-      <c r="J46" s="82"/>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
-      <c r="M46" s="82"/>
-      <c r="N46" s="82"/>
-      <c r="O46" s="82"/>
-      <c r="P46" s="82"/>
-      <c r="Q46" s="82"/>
-      <c r="R46" s="82"/>
-      <c r="S46" s="82"/>
-      <c r="T46" s="82"/>
-      <c r="U46" s="82"/>
-      <c r="V46" s="82"/>
-      <c r="W46" s="82"/>
-      <c r="X46" s="82"/>
-      <c r="Y46" s="82"/>
-      <c r="Z46" s="82"/>
-      <c r="AA46" s="82"/>
-      <c r="AB46" s="82"/>
-      <c r="AC46" s="82"/>
-      <c r="AD46" s="82"/>
-      <c r="AE46" s="82"/>
-      <c r="AF46" s="82"/>
-      <c r="AG46" s="82"/>
-      <c r="AH46" s="82"/>
-      <c r="AI46" s="82"/>
-      <c r="AJ46" s="82"/>
-      <c r="AK46" s="82"/>
-      <c r="AL46" s="82"/>
-      <c r="AM46" s="82"/>
-      <c r="AN46" s="82"/>
-      <c r="AO46" s="82"/>
-      <c r="AP46" s="82"/>
-      <c r="AQ46" s="82"/>
-      <c r="AR46" s="82"/>
-      <c r="AS46" s="82"/>
-      <c r="AT46" s="82"/>
-      <c r="AU46" s="82"/>
-      <c r="AV46" s="82"/>
-      <c r="AW46" s="82"/>
-      <c r="AX46" s="82"/>
-      <c r="AY46" s="82"/>
-      <c r="AZ46" s="82"/>
-      <c r="BA46" s="82"/>
-      <c r="BB46" s="82"/>
-      <c r="BC46" s="82"/>
-      <c r="BD46" s="82"/>
-      <c r="BE46" s="82"/>
-      <c r="BF46" s="82"/>
-      <c r="BG46" s="82"/>
-      <c r="BH46" s="82"/>
-      <c r="BI46" s="82"/>
-      <c r="BJ46" s="82"/>
-      <c r="BK46" s="82"/>
-      <c r="BL46" s="82"/>
-      <c r="BM46" s="82"/>
-      <c r="BN46" s="82"/>
-      <c r="BO46" s="82"/>
-      <c r="BP46" s="82"/>
-      <c r="BQ46" s="82"/>
-      <c r="BR46" s="82"/>
-      <c r="BS46" s="82"/>
-      <c r="BT46" s="82"/>
-      <c r="BU46" s="82"/>
-      <c r="BV46" s="82"/>
-      <c r="BW46" s="82"/>
-      <c r="BX46" s="82"/>
-      <c r="BY46" s="82"/>
-      <c r="BZ46" s="82"/>
-      <c r="CA46" s="82"/>
-      <c r="CB46" s="82"/>
-      <c r="CC46" s="82"/>
-      <c r="CD46" s="82"/>
-      <c r="CE46" s="82"/>
-      <c r="CF46" s="82"/>
-      <c r="CG46" s="82"/>
-      <c r="CH46" s="82"/>
-      <c r="CI46" s="82"/>
-      <c r="CJ46" s="82"/>
-      <c r="CK46" s="82"/>
-      <c r="CL46" s="82"/>
-      <c r="CM46" s="82"/>
-      <c r="CN46" s="82"/>
-      <c r="CO46" s="82"/>
-      <c r="CP46" s="82"/>
-      <c r="CQ46" s="82"/>
-      <c r="CR46" s="82"/>
-      <c r="CS46" s="82"/>
-      <c r="CT46" s="82"/>
-      <c r="CU46" s="82"/>
-      <c r="CV46" s="82"/>
-      <c r="CW46" s="82"/>
-      <c r="CX46" s="82"/>
-      <c r="CY46" s="82"/>
-      <c r="CZ46" s="82"/>
-      <c r="DA46" s="82"/>
-      <c r="DB46" s="82"/>
-      <c r="DC46" s="82"/>
-      <c r="DD46" s="82"/>
-      <c r="DE46" s="82"/>
-      <c r="DF46" s="82"/>
-      <c r="DG46" s="82"/>
-      <c r="DH46" s="82"/>
-      <c r="DI46" s="82"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="64"/>
+      <c r="M46" s="64"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="64"/>
+      <c r="P46" s="64"/>
+      <c r="Q46" s="64"/>
+      <c r="R46" s="64"/>
+      <c r="S46" s="64"/>
+      <c r="T46" s="64"/>
+      <c r="U46" s="64"/>
+      <c r="V46" s="64"/>
+      <c r="W46" s="64"/>
+      <c r="X46" s="64"/>
+      <c r="Y46" s="64"/>
+      <c r="Z46" s="64"/>
+      <c r="AA46" s="64"/>
+      <c r="AB46" s="64"/>
+      <c r="AC46" s="64"/>
+      <c r="AD46" s="64"/>
+      <c r="AE46" s="64"/>
+      <c r="AF46" s="64"/>
+      <c r="AG46" s="64"/>
+      <c r="AH46" s="64"/>
+      <c r="AI46" s="64"/>
+      <c r="AJ46" s="64"/>
+      <c r="AK46" s="64"/>
+      <c r="AL46" s="64"/>
+      <c r="AM46" s="64"/>
+      <c r="AN46" s="64"/>
+      <c r="AO46" s="64"/>
+      <c r="AP46" s="64"/>
+      <c r="AQ46" s="64"/>
+      <c r="AR46" s="64"/>
+      <c r="AS46" s="64"/>
+      <c r="AT46" s="64"/>
+      <c r="AU46" s="64"/>
+      <c r="AV46" s="64"/>
+      <c r="AW46" s="64"/>
+      <c r="AX46" s="64"/>
+      <c r="AY46" s="64"/>
+      <c r="AZ46" s="64"/>
+      <c r="BA46" s="64"/>
+      <c r="BB46" s="64"/>
+      <c r="BC46" s="64"/>
+      <c r="BD46" s="64"/>
+      <c r="BE46" s="64"/>
+      <c r="BF46" s="64"/>
+      <c r="BG46" s="64"/>
+      <c r="BH46" s="64"/>
+      <c r="BI46" s="64"/>
+      <c r="BJ46" s="64"/>
+      <c r="BK46" s="64"/>
+      <c r="BL46" s="64"/>
+      <c r="BM46" s="64"/>
+      <c r="BN46" s="64"/>
+      <c r="BO46" s="64"/>
+      <c r="BP46" s="64"/>
+      <c r="BQ46" s="64"/>
+      <c r="BR46" s="64"/>
+      <c r="BS46" s="64"/>
+      <c r="BT46" s="64"/>
+      <c r="BU46" s="64"/>
+      <c r="BV46" s="64"/>
+      <c r="BW46" s="64"/>
+      <c r="BX46" s="64"/>
+      <c r="BY46" s="64"/>
+      <c r="BZ46" s="64"/>
+      <c r="CA46" s="64"/>
+      <c r="CB46" s="64"/>
+      <c r="CC46" s="64"/>
+      <c r="CD46" s="64"/>
+      <c r="CE46" s="64"/>
+      <c r="CF46" s="64"/>
+      <c r="CG46" s="64"/>
+      <c r="CH46" s="64"/>
+      <c r="CI46" s="64"/>
+      <c r="CJ46" s="64"/>
+      <c r="CK46" s="64"/>
+      <c r="CL46" s="64"/>
+      <c r="CM46" s="64"/>
+      <c r="CN46" s="64"/>
+      <c r="CO46" s="64"/>
+      <c r="CP46" s="64"/>
+      <c r="CQ46" s="64"/>
+      <c r="CR46" s="64"/>
+      <c r="CS46" s="64"/>
+      <c r="CT46" s="64"/>
+      <c r="CU46" s="64"/>
+      <c r="CV46" s="64"/>
+      <c r="CW46" s="64"/>
+      <c r="CX46" s="64"/>
+      <c r="CY46" s="64"/>
+      <c r="CZ46" s="64"/>
+      <c r="DA46" s="64"/>
+      <c r="DB46" s="64"/>
+      <c r="DC46" s="64"/>
+      <c r="DD46" s="64"/>
+      <c r="DE46" s="64"/>
+      <c r="DF46" s="64"/>
+      <c r="DG46" s="64"/>
+      <c r="DH46" s="64"/>
+      <c r="DI46" s="64"/>
     </row>
     <row r="47" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -7167,116 +7197,146 @@
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="82"/>
-      <c r="M47" s="82"/>
-      <c r="N47" s="82"/>
-      <c r="O47" s="82"/>
-      <c r="P47" s="82"/>
-      <c r="Q47" s="82"/>
-      <c r="R47" s="82"/>
-      <c r="S47" s="82"/>
-      <c r="T47" s="82"/>
-      <c r="U47" s="82"/>
-      <c r="V47" s="82"/>
-      <c r="W47" s="82"/>
-      <c r="X47" s="82"/>
-      <c r="Y47" s="82"/>
-      <c r="Z47" s="82"/>
-      <c r="AA47" s="82"/>
-      <c r="AB47" s="82"/>
-      <c r="AC47" s="82"/>
-      <c r="AD47" s="82"/>
-      <c r="AE47" s="82"/>
-      <c r="AF47" s="82"/>
-      <c r="AG47" s="82"/>
-      <c r="AH47" s="82"/>
-      <c r="AI47" s="82"/>
-      <c r="AJ47" s="82"/>
-      <c r="AK47" s="82"/>
-      <c r="AL47" s="82"/>
-      <c r="AM47" s="82"/>
-      <c r="AN47" s="82"/>
-      <c r="AO47" s="82"/>
-      <c r="AP47" s="82"/>
-      <c r="AQ47" s="82"/>
-      <c r="AR47" s="82"/>
-      <c r="AS47" s="82"/>
-      <c r="AT47" s="82"/>
-      <c r="AU47" s="82"/>
-      <c r="AV47" s="82"/>
-      <c r="AW47" s="82"/>
-      <c r="AX47" s="82"/>
-      <c r="AY47" s="82"/>
-      <c r="AZ47" s="82"/>
-      <c r="BA47" s="82"/>
-      <c r="BB47" s="82"/>
-      <c r="BC47" s="82"/>
-      <c r="BD47" s="82"/>
-      <c r="BE47" s="82"/>
-      <c r="BF47" s="82"/>
-      <c r="BG47" s="82"/>
-      <c r="BH47" s="82"/>
-      <c r="BI47" s="82"/>
-      <c r="BJ47" s="82"/>
-      <c r="BK47" s="82"/>
-      <c r="BL47" s="82"/>
-      <c r="BM47" s="82"/>
-      <c r="BN47" s="82"/>
-      <c r="BO47" s="82"/>
-      <c r="BP47" s="82"/>
-      <c r="BQ47" s="82"/>
-      <c r="BR47" s="82"/>
-      <c r="BS47" s="82"/>
-      <c r="BT47" s="82"/>
-      <c r="BU47" s="82"/>
-      <c r="BV47" s="82"/>
-      <c r="BW47" s="82"/>
-      <c r="BX47" s="82"/>
-      <c r="BY47" s="82"/>
-      <c r="BZ47" s="82"/>
-      <c r="CA47" s="82"/>
-      <c r="CB47" s="82"/>
-      <c r="CC47" s="82"/>
-      <c r="CD47" s="82"/>
-      <c r="CE47" s="82"/>
-      <c r="CF47" s="82"/>
-      <c r="CG47" s="82"/>
-      <c r="CH47" s="82"/>
-      <c r="CI47" s="82"/>
-      <c r="CJ47" s="82"/>
-      <c r="CK47" s="82"/>
-      <c r="CL47" s="82"/>
-      <c r="CM47" s="82"/>
-      <c r="CN47" s="82"/>
-      <c r="CO47" s="82"/>
-      <c r="CP47" s="82"/>
-      <c r="CQ47" s="82"/>
-      <c r="CR47" s="82"/>
-      <c r="CS47" s="82"/>
-      <c r="CT47" s="82"/>
-      <c r="CU47" s="82"/>
-      <c r="CV47" s="82"/>
-      <c r="CW47" s="82"/>
-      <c r="CX47" s="82"/>
-      <c r="CY47" s="82"/>
-      <c r="CZ47" s="82"/>
-      <c r="DA47" s="82"/>
-      <c r="DB47" s="82"/>
-      <c r="DC47" s="82"/>
-      <c r="DD47" s="82"/>
-      <c r="DE47" s="82"/>
-      <c r="DF47" s="82"/>
-      <c r="DG47" s="82"/>
-      <c r="DH47" s="82"/>
-      <c r="DI47" s="82"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="64"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="64"/>
+      <c r="J47" s="64"/>
+      <c r="K47" s="64"/>
+      <c r="L47" s="64"/>
+      <c r="M47" s="64"/>
+      <c r="N47" s="64" t="str">
+        <f>IF(ISBLANK(D47),"",D47)</f>
+        <v/>
+      </c>
+      <c r="O47" s="64"/>
+      <c r="P47" s="64"/>
+      <c r="Q47" s="64"/>
+      <c r="R47" s="64"/>
+      <c r="S47" s="64"/>
+      <c r="T47" s="64"/>
+      <c r="U47" s="64"/>
+      <c r="V47" s="64"/>
+      <c r="W47" s="64"/>
+      <c r="X47" s="64" t="str">
+        <f t="shared" ref="X47" si="41">IF(ISBLANK(N47),"",N47)</f>
+        <v/>
+      </c>
+      <c r="Y47" s="64"/>
+      <c r="Z47" s="64"/>
+      <c r="AA47" s="64"/>
+      <c r="AB47" s="64"/>
+      <c r="AC47" s="64"/>
+      <c r="AD47" s="64"/>
+      <c r="AE47" s="64"/>
+      <c r="AF47" s="64"/>
+      <c r="AG47" s="64"/>
+      <c r="AH47" s="64" t="str">
+        <f t="shared" ref="AH47" si="42">IF(ISBLANK(X47),"",X47)</f>
+        <v/>
+      </c>
+      <c r="AI47" s="64"/>
+      <c r="AJ47" s="64"/>
+      <c r="AK47" s="64"/>
+      <c r="AL47" s="64"/>
+      <c r="AM47" s="64"/>
+      <c r="AN47" s="64"/>
+      <c r="AO47" s="64"/>
+      <c r="AP47" s="64"/>
+      <c r="AQ47" s="64"/>
+      <c r="AR47" s="64" t="str">
+        <f t="shared" ref="AR47" si="43">IF(ISBLANK(AH47),"",AH47)</f>
+        <v/>
+      </c>
+      <c r="AS47" s="64"/>
+      <c r="AT47" s="64"/>
+      <c r="AU47" s="64"/>
+      <c r="AV47" s="64"/>
+      <c r="AW47" s="64"/>
+      <c r="AX47" s="64"/>
+      <c r="AY47" s="64"/>
+      <c r="AZ47" s="64"/>
+      <c r="BA47" s="64"/>
+      <c r="BB47" s="64" t="str">
+        <f t="shared" ref="BB47" si="44">IF(ISBLANK(AR47),"",AR47)</f>
+        <v/>
+      </c>
+      <c r="BC47" s="64"/>
+      <c r="BD47" s="64"/>
+      <c r="BE47" s="64"/>
+      <c r="BF47" s="64"/>
+      <c r="BG47" s="64"/>
+      <c r="BH47" s="64"/>
+      <c r="BI47" s="64"/>
+      <c r="BJ47" s="64"/>
+      <c r="BK47" s="64"/>
+      <c r="BL47" s="64" t="str">
+        <f t="shared" ref="BL47" si="45">IF(ISBLANK(BB47),"",BB47)</f>
+        <v/>
+      </c>
+      <c r="BM47" s="64"/>
+      <c r="BN47" s="64"/>
+      <c r="BO47" s="64"/>
+      <c r="BP47" s="64"/>
+      <c r="BQ47" s="64"/>
+      <c r="BR47" s="64"/>
+      <c r="BS47" s="64"/>
+      <c r="BT47" s="64"/>
+      <c r="BU47" s="64"/>
+      <c r="BV47" s="64" t="str">
+        <f t="shared" ref="BV47" si="46">IF(ISBLANK(BL47),"",BL47)</f>
+        <v/>
+      </c>
+      <c r="BW47" s="64"/>
+      <c r="BX47" s="64"/>
+      <c r="BY47" s="64"/>
+      <c r="BZ47" s="64"/>
+      <c r="CA47" s="64"/>
+      <c r="CB47" s="64"/>
+      <c r="CC47" s="64"/>
+      <c r="CD47" s="64"/>
+      <c r="CE47" s="64"/>
+      <c r="CF47" s="64" t="str">
+        <f t="shared" ref="CF47" si="47">IF(ISBLANK(BV47),"",BV47)</f>
+        <v/>
+      </c>
+      <c r="CG47" s="64"/>
+      <c r="CH47" s="64"/>
+      <c r="CI47" s="64"/>
+      <c r="CJ47" s="64"/>
+      <c r="CK47" s="64"/>
+      <c r="CL47" s="64"/>
+      <c r="CM47" s="64"/>
+      <c r="CN47" s="64"/>
+      <c r="CO47" s="64"/>
+      <c r="CP47" s="64" t="str">
+        <f t="shared" ref="CP47" si="48">IF(ISBLANK(CF47),"",CF47)</f>
+        <v/>
+      </c>
+      <c r="CQ47" s="64"/>
+      <c r="CR47" s="64"/>
+      <c r="CS47" s="64"/>
+      <c r="CT47" s="64"/>
+      <c r="CU47" s="64"/>
+      <c r="CV47" s="64"/>
+      <c r="CW47" s="64"/>
+      <c r="CX47" s="64"/>
+      <c r="CY47" s="64"/>
+      <c r="CZ47" s="64" t="str">
+        <f t="shared" ref="CZ47" si="49">IF(ISBLANK(CP47),"",CP47)</f>
+        <v/>
+      </c>
+      <c r="DA47" s="64"/>
+      <c r="DB47" s="64"/>
+      <c r="DC47" s="64"/>
+      <c r="DD47" s="64"/>
+      <c r="DE47" s="64"/>
+      <c r="DF47" s="64"/>
+      <c r="DG47" s="64"/>
+      <c r="DH47" s="64"/>
+      <c r="DI47" s="64"/>
     </row>
     <row r="48" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
@@ -7284,558 +7344,464 @@
         <v>52</v>
       </c>
       <c r="C48" s="1"/>
-      <c r="D48" s="82"/>
-      <c r="E48" s="82"/>
-      <c r="F48" s="82"/>
-      <c r="G48" s="82"/>
-      <c r="H48" s="82"/>
-      <c r="I48" s="82"/>
-      <c r="J48" s="82"/>
-      <c r="K48" s="82"/>
-      <c r="L48" s="82"/>
-      <c r="M48" s="82"/>
-      <c r="N48" s="82"/>
-      <c r="O48" s="82"/>
-      <c r="P48" s="82"/>
-      <c r="Q48" s="82"/>
-      <c r="R48" s="82"/>
-      <c r="S48" s="82"/>
-      <c r="T48" s="82"/>
-      <c r="U48" s="82"/>
-      <c r="V48" s="82"/>
-      <c r="W48" s="82"/>
-      <c r="X48" s="82"/>
-      <c r="Y48" s="82"/>
-      <c r="Z48" s="82"/>
-      <c r="AA48" s="82"/>
-      <c r="AB48" s="82"/>
-      <c r="AC48" s="82"/>
-      <c r="AD48" s="82"/>
-      <c r="AE48" s="82"/>
-      <c r="AF48" s="82"/>
-      <c r="AG48" s="82"/>
-      <c r="AH48" s="82"/>
-      <c r="AI48" s="82"/>
-      <c r="AJ48" s="82"/>
-      <c r="AK48" s="82"/>
-      <c r="AL48" s="82"/>
-      <c r="AM48" s="82"/>
-      <c r="AN48" s="82"/>
-      <c r="AO48" s="82"/>
-      <c r="AP48" s="82"/>
-      <c r="AQ48" s="82"/>
-      <c r="AR48" s="82"/>
-      <c r="AS48" s="82"/>
-      <c r="AT48" s="82"/>
-      <c r="AU48" s="82"/>
-      <c r="AV48" s="82"/>
-      <c r="AW48" s="82"/>
-      <c r="AX48" s="82"/>
-      <c r="AY48" s="82"/>
-      <c r="AZ48" s="82"/>
-      <c r="BA48" s="82"/>
-      <c r="BB48" s="82"/>
-      <c r="BC48" s="82"/>
-      <c r="BD48" s="82"/>
-      <c r="BE48" s="82"/>
-      <c r="BF48" s="82"/>
-      <c r="BG48" s="82"/>
-      <c r="BH48" s="82"/>
-      <c r="BI48" s="82"/>
-      <c r="BJ48" s="82"/>
-      <c r="BK48" s="82"/>
-      <c r="BL48" s="82"/>
-      <c r="BM48" s="82"/>
-      <c r="BN48" s="82"/>
-      <c r="BO48" s="82"/>
-      <c r="BP48" s="82"/>
-      <c r="BQ48" s="82"/>
-      <c r="BR48" s="82"/>
-      <c r="BS48" s="82"/>
-      <c r="BT48" s="82"/>
-      <c r="BU48" s="82"/>
-      <c r="BV48" s="82"/>
-      <c r="BW48" s="82"/>
-      <c r="BX48" s="82"/>
-      <c r="BY48" s="82"/>
-      <c r="BZ48" s="82"/>
-      <c r="CA48" s="82"/>
-      <c r="CB48" s="82"/>
-      <c r="CC48" s="82"/>
-      <c r="CD48" s="82"/>
-      <c r="CE48" s="82"/>
-      <c r="CF48" s="82"/>
-      <c r="CG48" s="82"/>
-      <c r="CH48" s="82"/>
-      <c r="CI48" s="82"/>
-      <c r="CJ48" s="82"/>
-      <c r="CK48" s="82"/>
-      <c r="CL48" s="82"/>
-      <c r="CM48" s="82"/>
-      <c r="CN48" s="82"/>
-      <c r="CO48" s="82"/>
-      <c r="CP48" s="82"/>
-      <c r="CQ48" s="82"/>
-      <c r="CR48" s="82"/>
-      <c r="CS48" s="82"/>
-      <c r="CT48" s="82"/>
-      <c r="CU48" s="82"/>
-      <c r="CV48" s="82"/>
-      <c r="CW48" s="82"/>
-      <c r="CX48" s="82"/>
-      <c r="CY48" s="82"/>
-      <c r="CZ48" s="82"/>
-      <c r="DA48" s="82"/>
-      <c r="DB48" s="82"/>
-      <c r="DC48" s="82"/>
-      <c r="DD48" s="82"/>
-      <c r="DE48" s="82"/>
-      <c r="DF48" s="82"/>
-      <c r="DG48" s="82"/>
-      <c r="DH48" s="82"/>
-      <c r="DI48" s="82"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+      <c r="H48" s="64"/>
+      <c r="I48" s="64"/>
+      <c r="J48" s="64"/>
+      <c r="K48" s="64"/>
+      <c r="L48" s="64"/>
+      <c r="M48" s="64"/>
+      <c r="N48" s="64"/>
+      <c r="O48" s="64"/>
+      <c r="P48" s="64"/>
+      <c r="Q48" s="64"/>
+      <c r="R48" s="64"/>
+      <c r="S48" s="64"/>
+      <c r="T48" s="64"/>
+      <c r="U48" s="64"/>
+      <c r="V48" s="64"/>
+      <c r="W48" s="64"/>
+      <c r="X48" s="64"/>
+      <c r="Y48" s="64"/>
+      <c r="Z48" s="64"/>
+      <c r="AA48" s="64"/>
+      <c r="AB48" s="64"/>
+      <c r="AC48" s="64"/>
+      <c r="AD48" s="64"/>
+      <c r="AE48" s="64"/>
+      <c r="AF48" s="64"/>
+      <c r="AG48" s="64"/>
+      <c r="AH48" s="64"/>
+      <c r="AI48" s="64"/>
+      <c r="AJ48" s="64"/>
+      <c r="AK48" s="64"/>
+      <c r="AL48" s="64"/>
+      <c r="AM48" s="64"/>
+      <c r="AN48" s="64"/>
+      <c r="AO48" s="64"/>
+      <c r="AP48" s="64"/>
+      <c r="AQ48" s="64"/>
+      <c r="AR48" s="64"/>
+      <c r="AS48" s="64"/>
+      <c r="AT48" s="64"/>
+      <c r="AU48" s="64"/>
+      <c r="AV48" s="64"/>
+      <c r="AW48" s="64"/>
+      <c r="AX48" s="64"/>
+      <c r="AY48" s="64"/>
+      <c r="AZ48" s="64"/>
+      <c r="BA48" s="64"/>
+      <c r="BB48" s="64"/>
+      <c r="BC48" s="64"/>
+      <c r="BD48" s="64"/>
+      <c r="BE48" s="64"/>
+      <c r="BF48" s="64"/>
+      <c r="BG48" s="64"/>
+      <c r="BH48" s="64"/>
+      <c r="BI48" s="64"/>
+      <c r="BJ48" s="64"/>
+      <c r="BK48" s="64"/>
+      <c r="BL48" s="64"/>
+      <c r="BM48" s="64"/>
+      <c r="BN48" s="64"/>
+      <c r="BO48" s="64"/>
+      <c r="BP48" s="64"/>
+      <c r="BQ48" s="64"/>
+      <c r="BR48" s="64"/>
+      <c r="BS48" s="64"/>
+      <c r="BT48" s="64"/>
+      <c r="BU48" s="64"/>
+      <c r="BV48" s="64"/>
+      <c r="BW48" s="64"/>
+      <c r="BX48" s="64"/>
+      <c r="BY48" s="64"/>
+      <c r="BZ48" s="64"/>
+      <c r="CA48" s="64"/>
+      <c r="CB48" s="64"/>
+      <c r="CC48" s="64"/>
+      <c r="CD48" s="64"/>
+      <c r="CE48" s="64"/>
+      <c r="CF48" s="64"/>
+      <c r="CG48" s="64"/>
+      <c r="CH48" s="64"/>
+      <c r="CI48" s="64"/>
+      <c r="CJ48" s="64"/>
+      <c r="CK48" s="64"/>
+      <c r="CL48" s="64"/>
+      <c r="CM48" s="64"/>
+      <c r="CN48" s="64"/>
+      <c r="CO48" s="64"/>
+      <c r="CP48" s="64"/>
+      <c r="CQ48" s="64"/>
+      <c r="CR48" s="64"/>
+      <c r="CS48" s="64"/>
+      <c r="CT48" s="64"/>
+      <c r="CU48" s="64"/>
+      <c r="CV48" s="64"/>
+      <c r="CW48" s="64"/>
+      <c r="CX48" s="64"/>
+      <c r="CY48" s="64"/>
+      <c r="CZ48" s="64"/>
+      <c r="DA48" s="64"/>
+      <c r="DB48" s="64"/>
+      <c r="DC48" s="64"/>
+      <c r="DD48" s="64"/>
+      <c r="DE48" s="64"/>
+      <c r="DF48" s="64"/>
+      <c r="DG48" s="64"/>
+      <c r="DH48" s="64"/>
+      <c r="DI48" s="64"/>
     </row>
     <row r="49" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
-      <c r="D49" s="82"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="82"/>
-      <c r="G49" s="82"/>
-      <c r="H49" s="82"/>
-      <c r="I49" s="82"/>
-      <c r="J49" s="82"/>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
-      <c r="M49" s="82"/>
-      <c r="N49" s="82"/>
-      <c r="O49" s="82"/>
-      <c r="P49" s="82"/>
-      <c r="Q49" s="82"/>
-      <c r="R49" s="82"/>
-      <c r="S49" s="82"/>
-      <c r="T49" s="82"/>
-      <c r="U49" s="82"/>
-      <c r="V49" s="82"/>
-      <c r="W49" s="82"/>
-      <c r="X49" s="82"/>
-      <c r="Y49" s="82"/>
-      <c r="Z49" s="82"/>
-      <c r="AA49" s="82"/>
-      <c r="AB49" s="82"/>
-      <c r="AC49" s="82"/>
-      <c r="AD49" s="82"/>
-      <c r="AE49" s="82"/>
-      <c r="AF49" s="82"/>
-      <c r="AG49" s="82"/>
-      <c r="AH49" s="82"/>
-      <c r="AI49" s="82"/>
-      <c r="AJ49" s="82"/>
-      <c r="AK49" s="82"/>
-      <c r="AL49" s="82"/>
-      <c r="AM49" s="82"/>
-      <c r="AN49" s="82"/>
-      <c r="AO49" s="82"/>
-      <c r="AP49" s="82"/>
-      <c r="AQ49" s="82"/>
-      <c r="AR49" s="82"/>
-      <c r="AS49" s="82"/>
-      <c r="AT49" s="82"/>
-      <c r="AU49" s="82"/>
-      <c r="AV49" s="82"/>
-      <c r="AW49" s="82"/>
-      <c r="AX49" s="82"/>
-      <c r="AY49" s="82"/>
-      <c r="AZ49" s="82"/>
-      <c r="BA49" s="82"/>
-      <c r="BB49" s="82"/>
-      <c r="BC49" s="82"/>
-      <c r="BD49" s="82"/>
-      <c r="BE49" s="82"/>
-      <c r="BF49" s="82"/>
-      <c r="BG49" s="82"/>
-      <c r="BH49" s="82"/>
-      <c r="BI49" s="82"/>
-      <c r="BJ49" s="82"/>
-      <c r="BK49" s="82"/>
-      <c r="BL49" s="82"/>
-      <c r="BM49" s="82"/>
-      <c r="BN49" s="82"/>
-      <c r="BO49" s="82"/>
-      <c r="BP49" s="82"/>
-      <c r="BQ49" s="82"/>
-      <c r="BR49" s="82"/>
-      <c r="BS49" s="82"/>
-      <c r="BT49" s="82"/>
-      <c r="BU49" s="82"/>
-      <c r="BV49" s="82"/>
-      <c r="BW49" s="82"/>
-      <c r="BX49" s="82"/>
-      <c r="BY49" s="82"/>
-      <c r="BZ49" s="82"/>
-      <c r="CA49" s="82"/>
-      <c r="CB49" s="82"/>
-      <c r="CC49" s="82"/>
-      <c r="CD49" s="82"/>
-      <c r="CE49" s="82"/>
-      <c r="CF49" s="82"/>
-      <c r="CG49" s="82"/>
-      <c r="CH49" s="82"/>
-      <c r="CI49" s="82"/>
-      <c r="CJ49" s="82"/>
-      <c r="CK49" s="82"/>
-      <c r="CL49" s="82"/>
-      <c r="CM49" s="82"/>
-      <c r="CN49" s="82"/>
-      <c r="CO49" s="82"/>
-      <c r="CP49" s="82"/>
-      <c r="CQ49" s="82"/>
-      <c r="CR49" s="82"/>
-      <c r="CS49" s="82"/>
-      <c r="CT49" s="82"/>
-      <c r="CU49" s="82"/>
-      <c r="CV49" s="82"/>
-      <c r="CW49" s="82"/>
-      <c r="CX49" s="82"/>
-      <c r="CY49" s="82"/>
-      <c r="CZ49" s="82"/>
-      <c r="DA49" s="82"/>
-      <c r="DB49" s="82"/>
-      <c r="DC49" s="82"/>
-      <c r="DD49" s="82"/>
-      <c r="DE49" s="82"/>
-      <c r="DF49" s="82"/>
-      <c r="DG49" s="82"/>
-      <c r="DH49" s="82"/>
-      <c r="DI49" s="82"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="64"/>
+      <c r="F49" s="64"/>
+      <c r="G49" s="64"/>
+      <c r="H49" s="64"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="64"/>
+      <c r="K49" s="64"/>
+      <c r="L49" s="64"/>
+      <c r="M49" s="64"/>
+      <c r="N49" s="64"/>
+      <c r="O49" s="64"/>
+      <c r="P49" s="64"/>
+      <c r="Q49" s="64"/>
+      <c r="R49" s="64"/>
+      <c r="S49" s="64"/>
+      <c r="T49" s="64"/>
+      <c r="U49" s="64"/>
+      <c r="V49" s="64"/>
+      <c r="W49" s="64"/>
+      <c r="X49" s="64"/>
+      <c r="Y49" s="64"/>
+      <c r="Z49" s="64"/>
+      <c r="AA49" s="64"/>
+      <c r="AB49" s="64"/>
+      <c r="AC49" s="64"/>
+      <c r="AD49" s="64"/>
+      <c r="AE49" s="64"/>
+      <c r="AF49" s="64"/>
+      <c r="AG49" s="64"/>
+      <c r="AH49" s="64"/>
+      <c r="AI49" s="64"/>
+      <c r="AJ49" s="64"/>
+      <c r="AK49" s="64"/>
+      <c r="AL49" s="64"/>
+      <c r="AM49" s="64"/>
+      <c r="AN49" s="64"/>
+      <c r="AO49" s="64"/>
+      <c r="AP49" s="64"/>
+      <c r="AQ49" s="64"/>
+      <c r="AR49" s="64"/>
+      <c r="AS49" s="64"/>
+      <c r="AT49" s="64"/>
+      <c r="AU49" s="64"/>
+      <c r="AV49" s="64"/>
+      <c r="AW49" s="64"/>
+      <c r="AX49" s="64"/>
+      <c r="AY49" s="64"/>
+      <c r="AZ49" s="64"/>
+      <c r="BA49" s="64"/>
+      <c r="BB49" s="64"/>
+      <c r="BC49" s="64"/>
+      <c r="BD49" s="64"/>
+      <c r="BE49" s="64"/>
+      <c r="BF49" s="64"/>
+      <c r="BG49" s="64"/>
+      <c r="BH49" s="64"/>
+      <c r="BI49" s="64"/>
+      <c r="BJ49" s="64"/>
+      <c r="BK49" s="64"/>
+      <c r="BL49" s="64"/>
+      <c r="BM49" s="64"/>
+      <c r="BN49" s="64"/>
+      <c r="BO49" s="64"/>
+      <c r="BP49" s="64"/>
+      <c r="BQ49" s="64"/>
+      <c r="BR49" s="64"/>
+      <c r="BS49" s="64"/>
+      <c r="BT49" s="64"/>
+      <c r="BU49" s="64"/>
+      <c r="BV49" s="64"/>
+      <c r="BW49" s="64"/>
+      <c r="BX49" s="64"/>
+      <c r="BY49" s="64"/>
+      <c r="BZ49" s="64"/>
+      <c r="CA49" s="64"/>
+      <c r="CB49" s="64"/>
+      <c r="CC49" s="64"/>
+      <c r="CD49" s="64"/>
+      <c r="CE49" s="64"/>
+      <c r="CF49" s="64"/>
+      <c r="CG49" s="64"/>
+      <c r="CH49" s="64"/>
+      <c r="CI49" s="64"/>
+      <c r="CJ49" s="64"/>
+      <c r="CK49" s="64"/>
+      <c r="CL49" s="64"/>
+      <c r="CM49" s="64"/>
+      <c r="CN49" s="64"/>
+      <c r="CO49" s="64"/>
+      <c r="CP49" s="64"/>
+      <c r="CQ49" s="64"/>
+      <c r="CR49" s="64"/>
+      <c r="CS49" s="64"/>
+      <c r="CT49" s="64"/>
+      <c r="CU49" s="64"/>
+      <c r="CV49" s="64"/>
+      <c r="CW49" s="64"/>
+      <c r="CX49" s="64"/>
+      <c r="CY49" s="64"/>
+      <c r="CZ49" s="64"/>
+      <c r="DA49" s="64"/>
+      <c r="DB49" s="64"/>
+      <c r="DC49" s="64"/>
+      <c r="DD49" s="64"/>
+      <c r="DE49" s="64"/>
+      <c r="DF49" s="64"/>
+      <c r="DG49" s="64"/>
+      <c r="DH49" s="64"/>
+      <c r="DI49" s="64"/>
     </row>
     <row r="50" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
-      <c r="D50" s="82"/>
-      <c r="E50" s="82"/>
-      <c r="F50" s="82"/>
-      <c r="G50" s="82"/>
-      <c r="H50" s="82"/>
-      <c r="I50" s="82"/>
-      <c r="J50" s="82"/>
-      <c r="K50" s="82"/>
-      <c r="L50" s="82"/>
-      <c r="M50" s="82"/>
-      <c r="N50" s="82"/>
-      <c r="O50" s="82"/>
-      <c r="P50" s="82"/>
-      <c r="Q50" s="82"/>
-      <c r="R50" s="82"/>
-      <c r="S50" s="82"/>
-      <c r="T50" s="82"/>
-      <c r="U50" s="82"/>
-      <c r="V50" s="82"/>
-      <c r="W50" s="82"/>
-      <c r="X50" s="82"/>
-      <c r="Y50" s="82"/>
-      <c r="Z50" s="82"/>
-      <c r="AA50" s="82"/>
-      <c r="AB50" s="82"/>
-      <c r="AC50" s="82"/>
-      <c r="AD50" s="82"/>
-      <c r="AE50" s="82"/>
-      <c r="AF50" s="82"/>
-      <c r="AG50" s="82"/>
-      <c r="AH50" s="82"/>
-      <c r="AI50" s="82"/>
-      <c r="AJ50" s="82"/>
-      <c r="AK50" s="82"/>
-      <c r="AL50" s="82"/>
-      <c r="AM50" s="82"/>
-      <c r="AN50" s="82"/>
-      <c r="AO50" s="82"/>
-      <c r="AP50" s="82"/>
-      <c r="AQ50" s="82"/>
-      <c r="AR50" s="82"/>
-      <c r="AS50" s="82"/>
-      <c r="AT50" s="82"/>
-      <c r="AU50" s="82"/>
-      <c r="AV50" s="82"/>
-      <c r="AW50" s="82"/>
-      <c r="AX50" s="82"/>
-      <c r="AY50" s="82"/>
-      <c r="AZ50" s="82"/>
-      <c r="BA50" s="82"/>
-      <c r="BB50" s="82"/>
-      <c r="BC50" s="82"/>
-      <c r="BD50" s="82"/>
-      <c r="BE50" s="82"/>
-      <c r="BF50" s="82"/>
-      <c r="BG50" s="82"/>
-      <c r="BH50" s="82"/>
-      <c r="BI50" s="82"/>
-      <c r="BJ50" s="82"/>
-      <c r="BK50" s="82"/>
-      <c r="BL50" s="82"/>
-      <c r="BM50" s="82"/>
-      <c r="BN50" s="82"/>
-      <c r="BO50" s="82"/>
-      <c r="BP50" s="82"/>
-      <c r="BQ50" s="82"/>
-      <c r="BR50" s="82"/>
-      <c r="BS50" s="82"/>
-      <c r="BT50" s="82"/>
-      <c r="BU50" s="82"/>
-      <c r="BV50" s="82"/>
-      <c r="BW50" s="82"/>
-      <c r="BX50" s="82"/>
-      <c r="BY50" s="82"/>
-      <c r="BZ50" s="82"/>
-      <c r="CA50" s="82"/>
-      <c r="CB50" s="82"/>
-      <c r="CC50" s="82"/>
-      <c r="CD50" s="82"/>
-      <c r="CE50" s="82"/>
-      <c r="CF50" s="82"/>
-      <c r="CG50" s="82"/>
-      <c r="CH50" s="82"/>
-      <c r="CI50" s="82"/>
-      <c r="CJ50" s="82"/>
-      <c r="CK50" s="82"/>
-      <c r="CL50" s="82"/>
-      <c r="CM50" s="82"/>
-      <c r="CN50" s="82"/>
-      <c r="CO50" s="82"/>
-      <c r="CP50" s="82"/>
-      <c r="CQ50" s="82"/>
-      <c r="CR50" s="82"/>
-      <c r="CS50" s="82"/>
-      <c r="CT50" s="82"/>
-      <c r="CU50" s="82"/>
-      <c r="CV50" s="82"/>
-      <c r="CW50" s="82"/>
-      <c r="CX50" s="82"/>
-      <c r="CY50" s="82"/>
-      <c r="CZ50" s="82"/>
-      <c r="DA50" s="82"/>
-      <c r="DB50" s="82"/>
-      <c r="DC50" s="82"/>
-      <c r="DD50" s="82"/>
-      <c r="DE50" s="82"/>
-      <c r="DF50" s="82"/>
-      <c r="DG50" s="82"/>
-      <c r="DH50" s="82"/>
-      <c r="DI50" s="82"/>
+      <c r="D50" s="64"/>
+      <c r="E50" s="64"/>
+      <c r="F50" s="64"/>
+      <c r="G50" s="64"/>
+      <c r="H50" s="64"/>
+      <c r="I50" s="64"/>
+      <c r="J50" s="64"/>
+      <c r="K50" s="64"/>
+      <c r="L50" s="64"/>
+      <c r="M50" s="64"/>
+      <c r="N50" s="64"/>
+      <c r="O50" s="64"/>
+      <c r="P50" s="64"/>
+      <c r="Q50" s="64"/>
+      <c r="R50" s="64"/>
+      <c r="S50" s="64"/>
+      <c r="T50" s="64"/>
+      <c r="U50" s="64"/>
+      <c r="V50" s="64"/>
+      <c r="W50" s="64"/>
+      <c r="X50" s="64"/>
+      <c r="Y50" s="64"/>
+      <c r="Z50" s="64"/>
+      <c r="AA50" s="64"/>
+      <c r="AB50" s="64"/>
+      <c r="AC50" s="64"/>
+      <c r="AD50" s="64"/>
+      <c r="AE50" s="64"/>
+      <c r="AF50" s="64"/>
+      <c r="AG50" s="64"/>
+      <c r="AH50" s="64"/>
+      <c r="AI50" s="64"/>
+      <c r="AJ50" s="64"/>
+      <c r="AK50" s="64"/>
+      <c r="AL50" s="64"/>
+      <c r="AM50" s="64"/>
+      <c r="AN50" s="64"/>
+      <c r="AO50" s="64"/>
+      <c r="AP50" s="64"/>
+      <c r="AQ50" s="64"/>
+      <c r="AR50" s="64"/>
+      <c r="AS50" s="64"/>
+      <c r="AT50" s="64"/>
+      <c r="AU50" s="64"/>
+      <c r="AV50" s="64"/>
+      <c r="AW50" s="64"/>
+      <c r="AX50" s="64"/>
+      <c r="AY50" s="64"/>
+      <c r="AZ50" s="64"/>
+      <c r="BA50" s="64"/>
+      <c r="BB50" s="64"/>
+      <c r="BC50" s="64"/>
+      <c r="BD50" s="64"/>
+      <c r="BE50" s="64"/>
+      <c r="BF50" s="64"/>
+      <c r="BG50" s="64"/>
+      <c r="BH50" s="64"/>
+      <c r="BI50" s="64"/>
+      <c r="BJ50" s="64"/>
+      <c r="BK50" s="64"/>
+      <c r="BL50" s="64"/>
+      <c r="BM50" s="64"/>
+      <c r="BN50" s="64"/>
+      <c r="BO50" s="64"/>
+      <c r="BP50" s="64"/>
+      <c r="BQ50" s="64"/>
+      <c r="BR50" s="64"/>
+      <c r="BS50" s="64"/>
+      <c r="BT50" s="64"/>
+      <c r="BU50" s="64"/>
+      <c r="BV50" s="64"/>
+      <c r="BW50" s="64"/>
+      <c r="BX50" s="64"/>
+      <c r="BY50" s="64"/>
+      <c r="BZ50" s="64"/>
+      <c r="CA50" s="64"/>
+      <c r="CB50" s="64"/>
+      <c r="CC50" s="64"/>
+      <c r="CD50" s="64"/>
+      <c r="CE50" s="64"/>
+      <c r="CF50" s="64"/>
+      <c r="CG50" s="64"/>
+      <c r="CH50" s="64"/>
+      <c r="CI50" s="64"/>
+      <c r="CJ50" s="64"/>
+      <c r="CK50" s="64"/>
+      <c r="CL50" s="64"/>
+      <c r="CM50" s="64"/>
+      <c r="CN50" s="64"/>
+      <c r="CO50" s="64"/>
+      <c r="CP50" s="64"/>
+      <c r="CQ50" s="64"/>
+      <c r="CR50" s="64"/>
+      <c r="CS50" s="64"/>
+      <c r="CT50" s="64"/>
+      <c r="CU50" s="64"/>
+      <c r="CV50" s="64"/>
+      <c r="CW50" s="64"/>
+      <c r="CX50" s="64"/>
+      <c r="CY50" s="64"/>
+      <c r="CZ50" s="64"/>
+      <c r="DA50" s="64"/>
+      <c r="DB50" s="64"/>
+      <c r="DC50" s="64"/>
+      <c r="DD50" s="64"/>
+      <c r="DE50" s="64"/>
+      <c r="DF50" s="64"/>
+      <c r="DG50" s="64"/>
+      <c r="DH50" s="64"/>
+      <c r="DI50" s="64"/>
     </row>
     <row r="51" spans="1:113" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
-      <c r="D51" s="82"/>
-      <c r="E51" s="82"/>
-      <c r="F51" s="82"/>
-      <c r="G51" s="82"/>
-      <c r="H51" s="82"/>
-      <c r="I51" s="82"/>
-      <c r="J51" s="82"/>
-      <c r="K51" s="82"/>
-      <c r="L51" s="82"/>
-      <c r="M51" s="82"/>
-      <c r="N51" s="82"/>
-      <c r="O51" s="82"/>
-      <c r="P51" s="82"/>
-      <c r="Q51" s="82"/>
-      <c r="R51" s="82"/>
-      <c r="S51" s="82"/>
-      <c r="T51" s="82"/>
-      <c r="U51" s="82"/>
-      <c r="V51" s="82"/>
-      <c r="W51" s="82"/>
-      <c r="X51" s="82"/>
-      <c r="Y51" s="82"/>
-      <c r="Z51" s="82"/>
-      <c r="AA51" s="82"/>
-      <c r="AB51" s="82"/>
-      <c r="AC51" s="82"/>
-      <c r="AD51" s="82"/>
-      <c r="AE51" s="82"/>
-      <c r="AF51" s="82"/>
-      <c r="AG51" s="82"/>
-      <c r="AH51" s="82"/>
-      <c r="AI51" s="82"/>
-      <c r="AJ51" s="82"/>
-      <c r="AK51" s="82"/>
-      <c r="AL51" s="82"/>
-      <c r="AM51" s="82"/>
-      <c r="AN51" s="82"/>
-      <c r="AO51" s="82"/>
-      <c r="AP51" s="82"/>
-      <c r="AQ51" s="82"/>
-      <c r="AR51" s="82"/>
-      <c r="AS51" s="82"/>
-      <c r="AT51" s="82"/>
-      <c r="AU51" s="82"/>
-      <c r="AV51" s="82"/>
-      <c r="AW51" s="82"/>
-      <c r="AX51" s="82"/>
-      <c r="AY51" s="82"/>
-      <c r="AZ51" s="82"/>
-      <c r="BA51" s="82"/>
-      <c r="BB51" s="82"/>
-      <c r="BC51" s="82"/>
-      <c r="BD51" s="82"/>
-      <c r="BE51" s="82"/>
-      <c r="BF51" s="82"/>
-      <c r="BG51" s="82"/>
-      <c r="BH51" s="82"/>
-      <c r="BI51" s="82"/>
-      <c r="BJ51" s="82"/>
-      <c r="BK51" s="82"/>
-      <c r="BL51" s="82"/>
-      <c r="BM51" s="82"/>
-      <c r="BN51" s="82"/>
-      <c r="BO51" s="82"/>
-      <c r="BP51" s="82"/>
-      <c r="BQ51" s="82"/>
-      <c r="BR51" s="82"/>
-      <c r="BS51" s="82"/>
-      <c r="BT51" s="82"/>
-      <c r="BU51" s="82"/>
-      <c r="BV51" s="82"/>
-      <c r="BW51" s="82"/>
-      <c r="BX51" s="82"/>
-      <c r="BY51" s="82"/>
-      <c r="BZ51" s="82"/>
-      <c r="CA51" s="82"/>
-      <c r="CB51" s="82"/>
-      <c r="CC51" s="82"/>
-      <c r="CD51" s="82"/>
-      <c r="CE51" s="82"/>
-      <c r="CF51" s="82"/>
-      <c r="CG51" s="82"/>
-      <c r="CH51" s="82"/>
-      <c r="CI51" s="82"/>
-      <c r="CJ51" s="82"/>
-      <c r="CK51" s="82"/>
-      <c r="CL51" s="82"/>
-      <c r="CM51" s="82"/>
-      <c r="CN51" s="82"/>
-      <c r="CO51" s="82"/>
-      <c r="CP51" s="82"/>
-      <c r="CQ51" s="82"/>
-      <c r="CR51" s="82"/>
-      <c r="CS51" s="82"/>
-      <c r="CT51" s="82"/>
-      <c r="CU51" s="82"/>
-      <c r="CV51" s="82"/>
-      <c r="CW51" s="82"/>
-      <c r="CX51" s="82"/>
-      <c r="CY51" s="82"/>
-      <c r="CZ51" s="82"/>
-      <c r="DA51" s="82"/>
-      <c r="DB51" s="82"/>
-      <c r="DC51" s="82"/>
-      <c r="DD51" s="82"/>
-      <c r="DE51" s="82"/>
-      <c r="DF51" s="82"/>
-      <c r="DG51" s="82"/>
-      <c r="DH51" s="82"/>
-      <c r="DI51" s="82"/>
+      <c r="D51" s="64"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
+      <c r="H51" s="64"/>
+      <c r="I51" s="64"/>
+      <c r="J51" s="64"/>
+      <c r="K51" s="64"/>
+      <c r="L51" s="64"/>
+      <c r="M51" s="64"/>
+      <c r="N51" s="64"/>
+      <c r="O51" s="64"/>
+      <c r="P51" s="64"/>
+      <c r="Q51" s="64"/>
+      <c r="R51" s="64"/>
+      <c r="S51" s="64"/>
+      <c r="T51" s="64"/>
+      <c r="U51" s="64"/>
+      <c r="V51" s="64"/>
+      <c r="W51" s="64"/>
+      <c r="X51" s="64"/>
+      <c r="Y51" s="64"/>
+      <c r="Z51" s="64"/>
+      <c r="AA51" s="64"/>
+      <c r="AB51" s="64"/>
+      <c r="AC51" s="64"/>
+      <c r="AD51" s="64"/>
+      <c r="AE51" s="64"/>
+      <c r="AF51" s="64"/>
+      <c r="AG51" s="64"/>
+      <c r="AH51" s="64"/>
+      <c r="AI51" s="64"/>
+      <c r="AJ51" s="64"/>
+      <c r="AK51" s="64"/>
+      <c r="AL51" s="64"/>
+      <c r="AM51" s="64"/>
+      <c r="AN51" s="64"/>
+      <c r="AO51" s="64"/>
+      <c r="AP51" s="64"/>
+      <c r="AQ51" s="64"/>
+      <c r="AR51" s="64"/>
+      <c r="AS51" s="64"/>
+      <c r="AT51" s="64"/>
+      <c r="AU51" s="64"/>
+      <c r="AV51" s="64"/>
+      <c r="AW51" s="64"/>
+      <c r="AX51" s="64"/>
+      <c r="AY51" s="64"/>
+      <c r="AZ51" s="64"/>
+      <c r="BA51" s="64"/>
+      <c r="BB51" s="64"/>
+      <c r="BC51" s="64"/>
+      <c r="BD51" s="64"/>
+      <c r="BE51" s="64"/>
+      <c r="BF51" s="64"/>
+      <c r="BG51" s="64"/>
+      <c r="BH51" s="64"/>
+      <c r="BI51" s="64"/>
+      <c r="BJ51" s="64"/>
+      <c r="BK51" s="64"/>
+      <c r="BL51" s="64"/>
+      <c r="BM51" s="64"/>
+      <c r="BN51" s="64"/>
+      <c r="BO51" s="64"/>
+      <c r="BP51" s="64"/>
+      <c r="BQ51" s="64"/>
+      <c r="BR51" s="64"/>
+      <c r="BS51" s="64"/>
+      <c r="BT51" s="64"/>
+      <c r="BU51" s="64"/>
+      <c r="BV51" s="64"/>
+      <c r="BW51" s="64"/>
+      <c r="BX51" s="64"/>
+      <c r="BY51" s="64"/>
+      <c r="BZ51" s="64"/>
+      <c r="CA51" s="64"/>
+      <c r="CB51" s="64"/>
+      <c r="CC51" s="64"/>
+      <c r="CD51" s="64"/>
+      <c r="CE51" s="64"/>
+      <c r="CF51" s="64"/>
+      <c r="CG51" s="64"/>
+      <c r="CH51" s="64"/>
+      <c r="CI51" s="64"/>
+      <c r="CJ51" s="64"/>
+      <c r="CK51" s="64"/>
+      <c r="CL51" s="64"/>
+      <c r="CM51" s="64"/>
+      <c r="CN51" s="64"/>
+      <c r="CO51" s="64"/>
+      <c r="CP51" s="64"/>
+      <c r="CQ51" s="64"/>
+      <c r="CR51" s="64"/>
+      <c r="CS51" s="64"/>
+      <c r="CT51" s="64"/>
+      <c r="CU51" s="64"/>
+      <c r="CV51" s="64"/>
+      <c r="CW51" s="64"/>
+      <c r="CX51" s="64"/>
+      <c r="CY51" s="64"/>
+      <c r="CZ51" s="64"/>
+      <c r="DA51" s="64"/>
+      <c r="DB51" s="64"/>
+      <c r="DC51" s="64"/>
+      <c r="DD51" s="64"/>
+      <c r="DE51" s="64"/>
+      <c r="DF51" s="64"/>
+      <c r="DG51" s="64"/>
+      <c r="DH51" s="64"/>
+      <c r="DI51" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="111">
-    <mergeCell ref="CZ42:DI46"/>
-    <mergeCell ref="CZ47:DI51"/>
-    <mergeCell ref="BB42:BK46"/>
-    <mergeCell ref="BB47:BK51"/>
-    <mergeCell ref="BL42:BU46"/>
-    <mergeCell ref="BL47:BU51"/>
-    <mergeCell ref="BV42:CE46"/>
-    <mergeCell ref="BV47:CE51"/>
-    <mergeCell ref="CF42:CO46"/>
-    <mergeCell ref="CF47:CO51"/>
-    <mergeCell ref="CP42:CY46"/>
-    <mergeCell ref="CP47:CY51"/>
-    <mergeCell ref="D42:M46"/>
-    <mergeCell ref="D47:M51"/>
-    <mergeCell ref="N42:W46"/>
-    <mergeCell ref="N47:W51"/>
-    <mergeCell ref="X42:AG46"/>
-    <mergeCell ref="X47:AG51"/>
-    <mergeCell ref="AH42:AQ46"/>
-    <mergeCell ref="AH47:AQ51"/>
-    <mergeCell ref="AR42:BA46"/>
-    <mergeCell ref="AR47:BA51"/>
-    <mergeCell ref="CS6:CT6"/>
-    <mergeCell ref="CW6:CX6"/>
-    <mergeCell ref="DF2:DG3"/>
-    <mergeCell ref="DC6:DD6"/>
-    <mergeCell ref="DG6:DH6"/>
-    <mergeCell ref="CV2:CW3"/>
-    <mergeCell ref="CX2:CY3"/>
-    <mergeCell ref="CS4:CT4"/>
-    <mergeCell ref="CW4:CX4"/>
-    <mergeCell ref="CS5:CT5"/>
-    <mergeCell ref="CW5:CX5"/>
-    <mergeCell ref="DH2:DI3"/>
-    <mergeCell ref="DC4:DD4"/>
-    <mergeCell ref="DG4:DH4"/>
-    <mergeCell ref="DC5:DD5"/>
-    <mergeCell ref="DG5:DH5"/>
-    <mergeCell ref="BY6:BZ6"/>
-    <mergeCell ref="CC6:CD6"/>
-    <mergeCell ref="CL2:CM3"/>
-    <mergeCell ref="CN2:CO3"/>
-    <mergeCell ref="CI4:CJ4"/>
-    <mergeCell ref="CM4:CN4"/>
-    <mergeCell ref="CI5:CJ5"/>
-    <mergeCell ref="CM5:CN5"/>
-    <mergeCell ref="CI6:CJ6"/>
-    <mergeCell ref="CM6:CN6"/>
-    <mergeCell ref="CB2:CC3"/>
-    <mergeCell ref="CD2:CE3"/>
-    <mergeCell ref="BY4:BZ4"/>
-    <mergeCell ref="CC4:CD4"/>
-    <mergeCell ref="BY5:BZ5"/>
-    <mergeCell ref="CC5:CD5"/>
-    <mergeCell ref="BE6:BF6"/>
-    <mergeCell ref="BI6:BJ6"/>
-    <mergeCell ref="BR2:BS3"/>
-    <mergeCell ref="BT2:BU3"/>
-    <mergeCell ref="BO4:BP4"/>
-    <mergeCell ref="BS4:BT4"/>
-    <mergeCell ref="BO5:BP5"/>
-    <mergeCell ref="BS5:BT5"/>
-    <mergeCell ref="BO6:BP6"/>
-    <mergeCell ref="BS6:BT6"/>
-    <mergeCell ref="BH2:BI3"/>
-    <mergeCell ref="BJ2:BK3"/>
-    <mergeCell ref="BE4:BF4"/>
-    <mergeCell ref="BI4:BJ4"/>
-    <mergeCell ref="BE5:BF5"/>
-    <mergeCell ref="BI5:BJ5"/>
-    <mergeCell ref="AO6:AP6"/>
-    <mergeCell ref="AX2:AY3"/>
-    <mergeCell ref="AZ2:BA3"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AY4:AZ4"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AY5:AZ5"/>
-    <mergeCell ref="AU6:AV6"/>
-    <mergeCell ref="AY6:AZ6"/>
-    <mergeCell ref="AP2:AQ3"/>
-    <mergeCell ref="AN2:AO3"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="AE4:AF4"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AE6:AF6"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AD2:AE3"/>
-    <mergeCell ref="AF2:AG3"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK5:AL5"/>
     <mergeCell ref="U5:V5"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="U6:V6"/>
@@ -7853,6 +7819,100 @@
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="L2:M3"/>
     <mergeCell ref="G5:H5"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="AE4:AF4"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AE6:AF6"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AD2:AE3"/>
+    <mergeCell ref="AF2:AG3"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AO6:AP6"/>
+    <mergeCell ref="AX2:AY3"/>
+    <mergeCell ref="AZ2:BA3"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AY4:AZ4"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AY5:AZ5"/>
+    <mergeCell ref="AU6:AV6"/>
+    <mergeCell ref="AY6:AZ6"/>
+    <mergeCell ref="AP2:AQ3"/>
+    <mergeCell ref="AN2:AO3"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="BE6:BF6"/>
+    <mergeCell ref="BI6:BJ6"/>
+    <mergeCell ref="BR2:BS3"/>
+    <mergeCell ref="BT2:BU3"/>
+    <mergeCell ref="BO4:BP4"/>
+    <mergeCell ref="BS4:BT4"/>
+    <mergeCell ref="BO5:BP5"/>
+    <mergeCell ref="BS5:BT5"/>
+    <mergeCell ref="BO6:BP6"/>
+    <mergeCell ref="BS6:BT6"/>
+    <mergeCell ref="BH2:BI3"/>
+    <mergeCell ref="BJ2:BK3"/>
+    <mergeCell ref="BE4:BF4"/>
+    <mergeCell ref="BI4:BJ4"/>
+    <mergeCell ref="BE5:BF5"/>
+    <mergeCell ref="BI5:BJ5"/>
+    <mergeCell ref="BY6:BZ6"/>
+    <mergeCell ref="CC6:CD6"/>
+    <mergeCell ref="CL2:CM3"/>
+    <mergeCell ref="CN2:CO3"/>
+    <mergeCell ref="CI4:CJ4"/>
+    <mergeCell ref="CM4:CN4"/>
+    <mergeCell ref="CI5:CJ5"/>
+    <mergeCell ref="CM5:CN5"/>
+    <mergeCell ref="CI6:CJ6"/>
+    <mergeCell ref="CM6:CN6"/>
+    <mergeCell ref="CB2:CC3"/>
+    <mergeCell ref="CD2:CE3"/>
+    <mergeCell ref="BY4:BZ4"/>
+    <mergeCell ref="CC4:CD4"/>
+    <mergeCell ref="BY5:BZ5"/>
+    <mergeCell ref="CC5:CD5"/>
+    <mergeCell ref="CS6:CT6"/>
+    <mergeCell ref="CW6:CX6"/>
+    <mergeCell ref="DF2:DG3"/>
+    <mergeCell ref="DC6:DD6"/>
+    <mergeCell ref="DG6:DH6"/>
+    <mergeCell ref="CV2:CW3"/>
+    <mergeCell ref="CX2:CY3"/>
+    <mergeCell ref="CS4:CT4"/>
+    <mergeCell ref="CW4:CX4"/>
+    <mergeCell ref="CS5:CT5"/>
+    <mergeCell ref="CW5:CX5"/>
+    <mergeCell ref="DH2:DI3"/>
+    <mergeCell ref="DC4:DD4"/>
+    <mergeCell ref="DG4:DH4"/>
+    <mergeCell ref="DC5:DD5"/>
+    <mergeCell ref="DG5:DH5"/>
+    <mergeCell ref="D42:M46"/>
+    <mergeCell ref="D47:M51"/>
+    <mergeCell ref="N42:W46"/>
+    <mergeCell ref="N47:W51"/>
+    <mergeCell ref="X42:AG46"/>
+    <mergeCell ref="X47:AG51"/>
+    <mergeCell ref="AH42:AQ46"/>
+    <mergeCell ref="AH47:AQ51"/>
+    <mergeCell ref="AR42:BA46"/>
+    <mergeCell ref="AR47:BA51"/>
+    <mergeCell ref="CZ42:DI46"/>
+    <mergeCell ref="CZ47:DI51"/>
+    <mergeCell ref="BB42:BK46"/>
+    <mergeCell ref="BB47:BK51"/>
+    <mergeCell ref="BL42:BU46"/>
+    <mergeCell ref="BL47:BU51"/>
+    <mergeCell ref="BV42:CE46"/>
+    <mergeCell ref="BV47:CE51"/>
+    <mergeCell ref="CF42:CO46"/>
+    <mergeCell ref="CF47:CO51"/>
+    <mergeCell ref="CP42:CY46"/>
+    <mergeCell ref="CP47:CY51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -7870,9 +7930,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8038,26 +8101,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101401F0-266B-4560-B9EB-92F0EC712594}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2F065B-0021-4075-B51C-3CCB86F83471}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8081,9 +8133,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EB2F065B-0021-4075-B51C-3CCB86F83471}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{101401F0-266B-4560-B9EB-92F0EC712594}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="8fb9fcf7-a6bd-4cda-a801-5717a79e1e97"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>